<commit_message>
L36 closing the month
</commit_message>
<xml_diff>
--- a/msff/xls/assets{git.xlsx
+++ b/msff/xls/assets{git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0x\repos\repo1\msff\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB39093-931F-42F0-9EA1-1977409F4A7B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D59D91-032C-415B-AC96-2CA1A733D72D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="1950" windowWidth="21240" windowHeight="11835" tabRatio="673" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7156" uniqueCount="2897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7157" uniqueCount="2897">
   <si>
     <t>posb</t>
   </si>
@@ -9424,9 +9424,6 @@
     <t>Feb bonus ===</t>
   </si>
   <si>
-    <t>bx placeholder</t>
-  </si>
-  <si>
     <t>foods</t>
   </si>
   <si>
@@ -9436,9 +9433,6 @@
     <t>boy camp`</t>
   </si>
   <si>
-    <t>dental 26May</t>
-  </si>
-  <si>
     <t>boy NRIC</t>
   </si>
   <si>
@@ -9550,9 +9544,6 @@
     <t>7/11@T3 #boy</t>
   </si>
   <si>
-    <t>rmb109 pig trotters</t>
-  </si>
-  <si>
     <t>rmb144</t>
   </si>
   <si>
@@ -9562,10 +9553,19 @@
     <t>rmb101 JapMeal</t>
   </si>
   <si>
-    <t>rmbXXX</t>
-  </si>
-  <si>
     <t>cpf&gt;OC</t>
+  </si>
+  <si>
+    <t>rmbXXX HSBC</t>
+  </si>
+  <si>
+    <t>rmbXXX #104</t>
+  </si>
+  <si>
+    <t>rmb109# trotters</t>
+  </si>
+  <si>
+    <t>^10/6 AlipayDBS</t>
   </si>
 </sst>
 </file>
@@ -15315,7 +15315,7 @@
         <v>45000</v>
       </c>
       <c r="I22" s="63" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
@@ -33293,8 +33293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:JY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JM1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="JY14" sqref="JY14"/>
+    <sheetView tabSelected="1" topLeftCell="JN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="JX23" sqref="JX23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34427,14 +34427,14 @@
       </c>
       <c r="JU2" s="273">
         <f>JS2+JQ2-JW2</f>
-        <v>12027.001000000047</v>
+        <v>13504.421000000031</v>
       </c>
       <c r="JV2" s="760" t="s">
         <v>1911</v>
       </c>
       <c r="JW2" s="363">
         <f>SUM(JW3:JW27)</f>
-        <v>302908.67</v>
+        <v>301431.25</v>
       </c>
       <c r="JX2" s="608"/>
     </row>
@@ -35354,7 +35354,7 @@
         <v>7527.189000000023</v>
       </c>
       <c r="JP3" s="714" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="JQ3" s="203">
         <f>$IA$6</f>
@@ -35366,18 +35366,16 @@
       </c>
       <c r="JU3" s="273">
         <f>JU2-JS26-JS25</f>
-        <v>2736.7050000000486</v>
+        <v>4214.1250000000327</v>
       </c>
       <c r="JV3" s="782" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="JW3" s="203">
         <f>$IA$6</f>
         <v>-1.35</v>
       </c>
-      <c r="JX3" s="609">
-        <v>45086</v>
-      </c>
+      <c r="JX3" s="609"/>
     </row>
     <row r="4" spans="1:285" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="804" t="s">
@@ -35998,7 +35996,7 @@
       </c>
       <c r="JU4" s="286">
         <f>JU2-JU5</f>
-        <v>-0.58899999995082908</v>
+        <v>0.16100000003280002</v>
       </c>
       <c r="JV4" s="760" t="s">
         <v>2800</v>
@@ -36786,7 +36784,7 @@
         <v>-80000</v>
       </c>
       <c r="JR5" s="783" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="JS5" s="541">
         <v>-30</v>
@@ -36795,8 +36793,8 @@
         <v>352</v>
       </c>
       <c r="JU5" s="273">
-        <f>SUM(JU6:JU48)</f>
-        <v>12027.589999999998</v>
+        <f>SUM(JU6:JU49)</f>
+        <v>13504.259999999998</v>
       </c>
       <c r="JV5" s="765" t="s">
         <v>2679</v>
@@ -36805,7 +36803,7 @@
         <v>-77000</v>
       </c>
       <c r="JX5" s="609">
-        <v>45086</v>
+        <v>45093</v>
       </c>
     </row>
     <row r="6" spans="1:285" x14ac:dyDescent="0.2">
@@ -37579,10 +37577,10 @@
         <v>2664</v>
       </c>
       <c r="JS6" s="541" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="JT6" s="192" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="JU6" s="61">
         <v>2000</v>
@@ -38334,7 +38332,7 @@
         <v>64000</v>
       </c>
       <c r="JR7" s="783" t="s">
-        <v>2896</v>
+        <v>2892</v>
       </c>
       <c r="JS7" s="541">
         <v>236.43</v>
@@ -39056,9 +39054,11 @@
       </c>
       <c r="JS8" s="492"/>
       <c r="JT8" s="389" t="s">
-        <v>2849</v>
-      </c>
-      <c r="JU8" s="61"/>
+        <v>2112</v>
+      </c>
+      <c r="JU8" s="61">
+        <v>1476</v>
+      </c>
       <c r="JV8" s="320" t="s">
         <v>2467</v>
       </c>
@@ -39828,19 +39828,19 @@
         <v>31</v>
       </c>
       <c r="JR9" s="611" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="JS9" s="760">
         <v>2.33</v>
       </c>
       <c r="JT9" s="346" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="JU9" s="61">
         <v>10</v>
       </c>
       <c r="JV9" s="205" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="JW9" s="84">
         <v>0</v>
@@ -40559,13 +40559,13 @@
         <v>-1063</v>
       </c>
       <c r="JR10" s="611" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
       <c r="JS10" s="783">
         <v>3.4</v>
       </c>
       <c r="JT10" s="245" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="JU10" s="492">
         <v>1371.77</v>
@@ -41285,7 +41285,7 @@
         <v>52.000999999999998</v>
       </c>
       <c r="JN11" s="245" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="JO11" s="492">
         <v>1396.9</v>
@@ -41301,7 +41301,7 @@
       </c>
       <c r="JS11" s="514"/>
       <c r="JT11" s="245" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="JU11" s="492">
         <v>1478.09</v>
@@ -41312,7 +41312,9 @@
       <c r="JW11" s="268">
         <v>2600</v>
       </c>
-      <c r="JX11" s="608"/>
+      <c r="JX11" s="608">
+        <v>45093</v>
+      </c>
     </row>
     <row r="12" spans="1:285" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -41971,10 +41973,10 @@
         <v>2802</v>
       </c>
       <c r="JW12" s="268">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="JX12" s="608">
-        <v>45087</v>
+        <v>45093</v>
       </c>
       <c r="JY12" s="268"/>
     </row>
@@ -42664,10 +42666,10 @@
         <v>2803</v>
       </c>
       <c r="JW13" s="268">
-        <v>1952</v>
+        <v>597</v>
       </c>
       <c r="JX13" s="608">
-        <v>45087</v>
+        <v>45093</v>
       </c>
       <c r="JY13" s="268"/>
     </row>
@@ -43308,7 +43310,7 @@
         <v>966</v>
       </c>
       <c r="JL14" s="783" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="JM14" s="510">
         <v>1.96</v>
@@ -44054,7 +44056,7 @@
         <v>1556</v>
       </c>
       <c r="JL15" s="714" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="JM15" s="61">
         <f>25.72</f>
@@ -44073,7 +44075,7 @@
         <v>2441</v>
       </c>
       <c r="JR15" s="774" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="JS15" s="729">
         <v>200</v>
@@ -44766,7 +44768,7 @@
         <v>4000</v>
       </c>
       <c r="JL16" s="783" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="JM16" s="61">
         <f>180.39+64.94+57.72</f>
@@ -44783,7 +44785,7 @@
       </c>
       <c r="JQ16" s="607"/>
       <c r="JR16" s="800" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="JS16" s="729">
         <v>300</v>
@@ -45508,7 +45510,7 @@
         <v>0</v>
       </c>
       <c r="JR17" s="783" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="JS17" s="729">
         <v>2.95</v>
@@ -46192,7 +46194,7 @@
         <v>14</v>
       </c>
       <c r="JR18" s="10" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="JS18" s="793">
         <f>28.96</f>
@@ -46873,7 +46875,7 @@
         <v>210</v>
       </c>
       <c r="JR19" s="11" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="JS19" s="794">
         <f>183.29+65.98+58.65</f>
@@ -47566,13 +47568,13 @@
       </c>
       <c r="JQ20" s="2"/>
       <c r="JR20" s="11" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="JS20" s="795">
         <v>15.42</v>
       </c>
       <c r="JT20" s="345" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="JU20" s="203">
         <v>6.97</v>
@@ -48231,7 +48233,7 @@
         <v>1000</v>
       </c>
       <c r="JR21" s="796" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="JS21" s="797">
         <f>783.33+1167.38+1493.5+2179.3</f>
@@ -48891,11 +48893,11 @@
       </c>
       <c r="JQ22" s="2"/>
       <c r="JR22" s="796" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="JS22" s="797"/>
       <c r="JT22" s="337" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
       <c r="JU22" s="61">
         <v>10</v>
@@ -49516,7 +49518,7 @@
       <c r="JR23" s="770"/>
       <c r="JS23" s="510"/>
       <c r="JT23" s="337" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="JU23" s="61">
         <v>48.2</v>
@@ -50100,13 +50102,13 @@
       </c>
       <c r="JS24" s="758"/>
       <c r="JT24" s="337" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="JU24" s="61">
         <v>68.900000000000006</v>
       </c>
       <c r="JV24" s="768" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="JW24" s="61">
         <v>453.6</v>
@@ -50670,7 +50672,7 @@
         <v>3900.06</v>
       </c>
       <c r="JT25" s="337" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="JU25" s="61">
         <v>41.5</v>
@@ -51194,24 +51196,20 @@
       </c>
       <c r="JQ26" s="2"/>
       <c r="JR26" s="388" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="JS26" s="273">
         <f>SUM(JU10:JU12)</f>
         <v>5390.235999999999</v>
       </c>
       <c r="JT26" s="337" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="JU26" s="533">
         <v>11</v>
       </c>
-      <c r="JV26" s="772" t="s">
-        <v>2853</v>
-      </c>
-      <c r="JW26" s="61">
-        <v>120.42</v>
-      </c>
+      <c r="JV26" s="772"/>
+      <c r="JW26" s="61"/>
       <c r="JY26" s="268"/>
     </row>
     <row r="27" spans="1:285" x14ac:dyDescent="0.2">
@@ -51769,7 +51767,7 @@
         <v>59.4</v>
       </c>
       <c r="JL27" s="388" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="JM27" s="273">
         <f>SUM(JO11:JO13)</f>
@@ -51788,7 +51786,7 @@
       </c>
       <c r="JS27" s="2">
         <f>SUM(JU8:JU8)</f>
-        <v>0</v>
+        <v>1476</v>
       </c>
       <c r="JT27" s="760" t="s">
         <v>2718</v>
@@ -53996,7 +53994,7 @@
         <v>30</v>
       </c>
       <c r="JU31" s="543" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="JV31" s="760" t="s">
         <v>1034</v>
@@ -54935,7 +54933,7 @@
         <v>2792</v>
       </c>
       <c r="JR33" s="341" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="JS33" s="353">
         <v>100</v>
@@ -54944,7 +54942,7 @@
         <v>10</v>
       </c>
       <c r="JU33" s="543" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="JY33" s="760"/>
     </row>
@@ -55360,7 +55358,7 @@
         <v>10</v>
       </c>
       <c r="JU34" s="543" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="JV34" s="760" t="s">
         <v>2767</v>
@@ -55748,7 +55746,7 @@
         <v>93</v>
       </c>
       <c r="JT35" s="760" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="JU35" s="533">
         <v>139</v>
@@ -56084,7 +56082,7 @@
         <v>1034</v>
       </c>
       <c r="JT36" s="799" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="JU36" s="533">
         <v>5.38</v>
@@ -56427,7 +56425,7 @@
       </c>
       <c r="JS37" s="494"/>
       <c r="JT37" s="784" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="JU37" s="785">
         <v>2.2000000000000002</v>
@@ -56732,7 +56730,7 @@
       </c>
       <c r="JS38" s="494"/>
       <c r="JT38" s="789" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="JU38" s="787">
         <v>89.39</v>
@@ -57032,10 +57030,10 @@
         <v>2787</v>
       </c>
       <c r="JS39" s="792" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="JT39" s="786" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="JU39" s="787">
         <f>69.93+136.83</f>
@@ -57321,7 +57319,7 @@
       <c r="JP40" s="748"/>
       <c r="JQ40" s="748"/>
       <c r="JT40" s="788" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="JU40" s="787">
         <v>18.8</v>
@@ -57489,7 +57487,7 @@
       <c r="JR41" s="760"/>
       <c r="JS41" s="760"/>
       <c r="JT41" s="789" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="JU41" s="787">
         <v>89.8</v>
@@ -58210,10 +58208,10 @@
         <v>120.36</v>
       </c>
       <c r="JT44" s="202" t="s">
-        <v>2891</v>
+        <v>2895</v>
       </c>
       <c r="JU44" s="357">
-        <v>20.6</v>
+        <v>21.27</v>
       </c>
     </row>
     <row r="45" spans="1:285" x14ac:dyDescent="0.2">
@@ -58400,12 +58398,10 @@
       <c r="JO45" s="533">
         <v>2.79</v>
       </c>
-      <c r="JT45" s="400" t="s">
-        <v>2892</v>
-      </c>
-      <c r="JU45" s="533">
-        <v>27.83</v>
-      </c>
+      <c r="JT45" s="202" t="s">
+        <v>2896</v>
+      </c>
+      <c r="JU45" s="357"/>
     </row>
     <row r="46" spans="1:285" x14ac:dyDescent="0.2">
       <c r="AO46" s="142" t="s">
@@ -58573,10 +58569,10 @@
         <v>8.5500000000000007</v>
       </c>
       <c r="JT46" s="400" t="s">
-        <v>2893</v>
+        <v>2889</v>
       </c>
       <c r="JU46" s="533">
-        <v>8.61</v>
+        <v>27.83</v>
       </c>
     </row>
     <row r="47" spans="1:285" x14ac:dyDescent="0.2">
@@ -58711,10 +58707,10 @@
         <v>10.35</v>
       </c>
       <c r="JT47" s="400" t="s">
-        <v>2894</v>
+        <v>2890</v>
       </c>
       <c r="JU47" s="533">
-        <v>19.46</v>
+        <v>8.61</v>
       </c>
     </row>
     <row r="48" spans="1:285" x14ac:dyDescent="0.2">
@@ -58871,11 +58867,10 @@
         <v>15.000999999999999</v>
       </c>
       <c r="JT48" s="400" t="s">
-        <v>2895</v>
-      </c>
-      <c r="JU48" s="357">
-        <f>5.42+0.41+0.58+2.33+0.29+0.28+0.26+1.45+0.29+4.73+1.54</f>
-        <v>17.579999999999998</v>
+        <v>2891</v>
+      </c>
+      <c r="JU48" s="533">
+        <v>19.46</v>
       </c>
     </row>
     <row r="49" spans="41:283" x14ac:dyDescent="0.2">
@@ -59003,6 +58998,13 @@
       <c r="JO49" s="357">
         <v>7.67</v>
       </c>
+      <c r="JT49" s="400" t="s">
+        <v>2893</v>
+      </c>
+      <c r="JU49" s="357">
+        <f>5.42+0.41+0.58+2.33+0.29+0.28+0.26+1.45+0.29+4.73+1.54</f>
+        <v>17.579999999999998</v>
+      </c>
     </row>
     <row r="50" spans="41:283" x14ac:dyDescent="0.2">
       <c r="AO50" s="142" t="s">
@@ -59128,6 +59130,13 @@
       </c>
       <c r="JO50" s="357">
         <v>3</v>
+      </c>
+      <c r="JT50" s="400" t="s">
+        <v>2894</v>
+      </c>
+      <c r="JU50" s="760">
+        <f>0.29*3</f>
+        <v>0.86999999999999988</v>
       </c>
     </row>
     <row r="51" spans="41:283" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Acer950 EGA | rbbt
</commit_message>
<xml_diff>
--- a/msff/xls/assets{git.xlsx
+++ b/msff/xls/assets{git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0x\repo1\msff\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA518155-56C0-47D9-ADD3-A6120E8A6316}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FD55AB-B9BC-4FF4-A99E-E62D1DD468FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1230" yWindow="2355" windowWidth="16185" windowHeight="11835" tabRatio="673" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,7 +769,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8558" uniqueCount="3515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8558" uniqueCount="3516">
   <si>
     <t>sigma1(15dec2002)=</t>
   </si>
@@ -11493,6 +11493,9 @@
   </si>
   <si>
     <t xml:space="preserve">scsc @ACL↴ </t>
+  </si>
+  <si>
+    <t>{RBBT</t>
   </si>
 </sst>
 </file>
@@ -13482,69 +13485,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -13562,10 +13502,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -13580,20 +13596,71 @@
     <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -13613,70 +13680,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="39" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18308,109 +18311,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:63">
-      <c r="B1" s="661" t="s">
+      <c r="B1" s="686" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="661"/>
-      <c r="D1" s="662" t="s">
+      <c r="C1" s="686"/>
+      <c r="D1" s="687" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="661"/>
-      <c r="F1" s="662" t="s">
+      <c r="E1" s="686"/>
+      <c r="F1" s="687" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="661"/>
-      <c r="H1" s="663" t="s">
+      <c r="G1" s="686"/>
+      <c r="H1" s="685" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="663"/>
-      <c r="J1" s="664" t="s">
+      <c r="I1" s="685"/>
+      <c r="J1" s="679" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="665"/>
-      <c r="L1" s="666" t="s">
+      <c r="K1" s="680"/>
+      <c r="L1" s="683" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="667"/>
-      <c r="N1" s="663" t="s">
+      <c r="M1" s="684"/>
+      <c r="N1" s="685" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="663"/>
-      <c r="P1" s="664" t="s">
+      <c r="O1" s="685"/>
+      <c r="P1" s="679" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="665"/>
-      <c r="R1" s="666" t="s">
+      <c r="Q1" s="680"/>
+      <c r="R1" s="683" t="s">
         <v>98</v>
       </c>
-      <c r="S1" s="667"/>
-      <c r="T1" s="668" t="s">
+      <c r="S1" s="684"/>
+      <c r="T1" s="669" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="668"/>
-      <c r="V1" s="664" t="s">
+      <c r="U1" s="669"/>
+      <c r="V1" s="679" t="s">
         <v>92</v>
       </c>
-      <c r="W1" s="665"/>
-      <c r="X1" s="669" t="s">
+      <c r="W1" s="680"/>
+      <c r="X1" s="675" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="670"/>
-      <c r="Z1" s="668" t="s">
+      <c r="Y1" s="676"/>
+      <c r="Z1" s="669" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="668"/>
-      <c r="AB1" s="671" t="s">
+      <c r="AA1" s="669"/>
+      <c r="AB1" s="673" t="s">
         <v>92</v>
       </c>
-      <c r="AC1" s="672"/>
-      <c r="AD1" s="673" t="s">
+      <c r="AC1" s="674"/>
+      <c r="AD1" s="681" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" s="674"/>
-      <c r="AF1" s="668" t="s">
+      <c r="AE1" s="682"/>
+      <c r="AF1" s="669" t="s">
         <v>102</v>
       </c>
-      <c r="AG1" s="668"/>
-      <c r="AH1" s="671" t="s">
+      <c r="AG1" s="669"/>
+      <c r="AH1" s="673" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" s="672"/>
-      <c r="AJ1" s="669" t="s">
+      <c r="AI1" s="674"/>
+      <c r="AJ1" s="675" t="s">
         <v>103</v>
       </c>
-      <c r="AK1" s="670"/>
-      <c r="AL1" s="668" t="s">
+      <c r="AK1" s="676"/>
+      <c r="AL1" s="669" t="s">
         <v>104</v>
       </c>
-      <c r="AM1" s="668"/>
-      <c r="AN1" s="675" t="s">
+      <c r="AM1" s="669"/>
+      <c r="AN1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="AO1" s="676"/>
-      <c r="AP1" s="677" t="s">
+      <c r="AO1" s="678"/>
+      <c r="AP1" s="667" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="678"/>
-      <c r="AR1" s="668" t="s">
+      <c r="AQ1" s="668"/>
+      <c r="AR1" s="669" t="s">
         <v>106</v>
       </c>
-      <c r="AS1" s="668"/>
-      <c r="AV1" s="677" t="s">
+      <c r="AS1" s="669"/>
+      <c r="AV1" s="667" t="s">
         <v>107</v>
       </c>
-      <c r="AW1" s="678"/>
-      <c r="AX1" s="679" t="s">
+      <c r="AW1" s="668"/>
+      <c r="AX1" s="670" t="s">
         <v>108</v>
       </c>
-      <c r="AY1" s="679"/>
-      <c r="AZ1" s="679"/>
+      <c r="AY1" s="670"/>
+      <c r="AZ1" s="670"/>
       <c r="BA1" s="354"/>
-      <c r="BB1" s="680">
+      <c r="BB1" s="671">
         <v>42942</v>
       </c>
-      <c r="BC1" s="681"/>
-      <c r="BD1" s="681"/>
+      <c r="BC1" s="672"/>
+      <c r="BD1" s="672"/>
     </row>
     <row r="2" spans="2:63" ht="3.75" customHeight="1">
       <c r="H2" s="9"/>
@@ -18618,10 +18621,10 @@
         <f>S3-S5</f>
         <v>33.727079999938724</v>
       </c>
-      <c r="T4" s="687" t="s">
+      <c r="T4" s="666" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="687"/>
+      <c r="U4" s="666"/>
       <c r="X4" s="435" t="s">
         <v>123</v>
       </c>
@@ -18629,10 +18632,10 @@
         <f>Y3-Y6</f>
         <v>4.9669099999591708</v>
       </c>
-      <c r="Z4" s="687" t="s">
+      <c r="Z4" s="666" t="s">
         <v>125</v>
       </c>
-      <c r="AA4" s="687"/>
+      <c r="AA4" s="666"/>
       <c r="AD4" s="404" t="s">
         <v>123</v>
       </c>
@@ -18640,10 +18643,10 @@
         <f>AE3-AE5</f>
         <v>-52.526899999851594</v>
       </c>
-      <c r="AF4" s="687" t="s">
+      <c r="AF4" s="666" t="s">
         <v>125</v>
       </c>
-      <c r="AG4" s="687"/>
+      <c r="AG4" s="666"/>
       <c r="AH4" s="72"/>
       <c r="AI4" s="72"/>
       <c r="AJ4" s="404" t="s">
@@ -18653,10 +18656,10 @@
         <f>AK3-AK5</f>
         <v>94.988909999992757</v>
       </c>
-      <c r="AL4" s="687" t="s">
+      <c r="AL4" s="666" t="s">
         <v>125</v>
       </c>
-      <c r="AM4" s="687"/>
+      <c r="AM4" s="666"/>
       <c r="AP4" s="58" t="s">
         <v>123</v>
       </c>
@@ -18664,18 +18667,18 @@
         <f>AQ3-AQ5</f>
         <v>33.841989999942598</v>
       </c>
-      <c r="AR4" s="687" t="s">
+      <c r="AR4" s="666" t="s">
         <v>125</v>
       </c>
-      <c r="AS4" s="687"/>
-      <c r="AX4" s="687" t="s">
+      <c r="AS4" s="666"/>
+      <c r="AX4" s="666" t="s">
         <v>126</v>
       </c>
-      <c r="AY4" s="687"/>
-      <c r="BB4" s="687" t="s">
+      <c r="AY4" s="666"/>
+      <c r="BB4" s="666" t="s">
         <v>127</v>
       </c>
-      <c r="BC4" s="687"/>
+      <c r="BC4" s="666"/>
     </row>
     <row r="5" spans="2:63" ht="39" customHeight="1">
       <c r="B5" t="s">
@@ -18720,8 +18723,8 @@
         <f>SUM(S15:S55)</f>
         <v>104150.52223000005</v>
       </c>
-      <c r="T5" s="687"/>
-      <c r="U5" s="687"/>
+      <c r="T5" s="666"/>
+      <c r="U5" s="666"/>
       <c r="V5" s="348" t="s">
         <v>132</v>
       </c>
@@ -18729,8 +18732,8 @@
         <v>2050</v>
       </c>
       <c r="X5" s="409"/>
-      <c r="Z5" s="687"/>
-      <c r="AA5" s="687"/>
+      <c r="Z5" s="666"/>
+      <c r="AA5" s="666"/>
       <c r="AB5" s="72" t="s">
         <v>133</v>
       </c>
@@ -18744,8 +18747,8 @@
         <f>SUM(AE11:AE55)</f>
         <v>224043.01899999983</v>
       </c>
-      <c r="AF5" s="687"/>
-      <c r="AG5" s="687"/>
+      <c r="AF5" s="666"/>
+      <c r="AG5" s="666"/>
       <c r="AH5" s="72"/>
       <c r="AI5" s="72"/>
       <c r="AJ5" s="404" t="s">
@@ -18755,8 +18758,8 @@
         <f>SUM(AK11:AK59)</f>
         <v>30858.011000000002</v>
       </c>
-      <c r="AL5" s="687"/>
-      <c r="AM5" s="687"/>
+      <c r="AL5" s="666"/>
+      <c r="AM5" s="666"/>
       <c r="AN5" s="406" t="s">
         <v>135</v>
       </c>
@@ -18770,22 +18773,22 @@
         <f>SUM(AQ11:AQ82)</f>
         <v>102060.80700000007</v>
       </c>
-      <c r="AR5" s="687"/>
-      <c r="AS5" s="687"/>
-      <c r="AX5" s="687"/>
-      <c r="AY5" s="687"/>
-      <c r="BB5" s="687"/>
-      <c r="BC5" s="687"/>
-      <c r="BD5" s="682" t="s">
+      <c r="AR5" s="666"/>
+      <c r="AS5" s="666"/>
+      <c r="AX5" s="666"/>
+      <c r="AY5" s="666"/>
+      <c r="BB5" s="666"/>
+      <c r="BC5" s="666"/>
+      <c r="BD5" s="661" t="s">
         <v>136</v>
       </c>
-      <c r="BE5" s="682"/>
-      <c r="BF5" s="682"/>
-      <c r="BG5" s="682"/>
-      <c r="BH5" s="682"/>
-      <c r="BI5" s="682"/>
-      <c r="BJ5" s="682"/>
-      <c r="BK5" s="682"/>
+      <c r="BE5" s="661"/>
+      <c r="BF5" s="661"/>
+      <c r="BG5" s="661"/>
+      <c r="BH5" s="661"/>
+      <c r="BI5" s="661"/>
+      <c r="BJ5" s="661"/>
+      <c r="BK5" s="661"/>
     </row>
     <row r="6" spans="2:63" ht="25.5">
       <c r="B6" t="s">
@@ -20679,10 +20682,10 @@
       <c r="T23" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="V23" s="683" t="s">
+      <c r="V23" s="662" t="s">
         <v>335</v>
       </c>
-      <c r="W23" s="684"/>
+      <c r="W23" s="663"/>
       <c r="X23" s="561" t="s">
         <v>336</v>
       </c>
@@ -20764,8 +20767,8 @@
       <c r="T24" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="V24" s="685"/>
-      <c r="W24" s="686"/>
+      <c r="V24" s="664"/>
+      <c r="W24" s="665"/>
       <c r="X24" s="561" t="s">
         <v>342</v>
       </c>
@@ -22625,6 +22628,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BB1:BD1"/>
     <mergeCell ref="BD5:BK5"/>
     <mergeCell ref="V23:W24"/>
     <mergeCell ref="T4:U5"/>
@@ -22634,31 +22662,6 @@
     <mergeCell ref="AR4:AS5"/>
     <mergeCell ref="AX4:AY5"/>
     <mergeCell ref="BB4:BC5"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -24677,318 +24680,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:162" ht="18">
-      <c r="B1" s="661" t="s">
+      <c r="B1" s="686" t="s">
         <v>567</v>
       </c>
-      <c r="C1" s="661"/>
-      <c r="D1" s="673" t="s">
+      <c r="C1" s="686"/>
+      <c r="D1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="E1" s="674"/>
-      <c r="F1" s="661" t="s">
+      <c r="E1" s="682"/>
+      <c r="F1" s="686" t="s">
         <v>569</v>
       </c>
-      <c r="G1" s="661"/>
-      <c r="H1" s="690" t="s">
+      <c r="G1" s="686"/>
+      <c r="H1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="I1" s="691"/>
-      <c r="J1" s="673" t="s">
+      <c r="I1" s="696"/>
+      <c r="J1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="K1" s="674"/>
-      <c r="L1" s="661" t="s">
+      <c r="K1" s="682"/>
+      <c r="L1" s="686" t="s">
         <v>571</v>
       </c>
-      <c r="M1" s="661"/>
-      <c r="N1" s="690" t="s">
+      <c r="M1" s="686"/>
+      <c r="N1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="O1" s="691"/>
-      <c r="P1" s="673" t="s">
+      <c r="O1" s="696"/>
+      <c r="P1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="Q1" s="674"/>
-      <c r="R1" s="661" t="s">
+      <c r="Q1" s="682"/>
+      <c r="R1" s="686" t="s">
         <v>572</v>
       </c>
-      <c r="S1" s="661"/>
-      <c r="T1" s="690" t="s">
+      <c r="S1" s="686"/>
+      <c r="T1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="U1" s="691"/>
-      <c r="V1" s="673" t="s">
+      <c r="U1" s="696"/>
+      <c r="V1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="W1" s="674"/>
-      <c r="X1" s="661" t="s">
+      <c r="W1" s="682"/>
+      <c r="X1" s="686" t="s">
         <v>573</v>
       </c>
-      <c r="Y1" s="661"/>
-      <c r="Z1" s="690" t="s">
+      <c r="Y1" s="686"/>
+      <c r="Z1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="AA1" s="691"/>
-      <c r="AB1" s="673" t="s">
+      <c r="AA1" s="696"/>
+      <c r="AB1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="AC1" s="674"/>
-      <c r="AD1" s="661" t="s">
+      <c r="AC1" s="682"/>
+      <c r="AD1" s="686" t="s">
         <v>574</v>
       </c>
-      <c r="AE1" s="661"/>
-      <c r="AF1" s="690" t="s">
+      <c r="AE1" s="686"/>
+      <c r="AF1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="AG1" s="691"/>
-      <c r="AH1" s="673" t="s">
+      <c r="AG1" s="696"/>
+      <c r="AH1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="AI1" s="674"/>
-      <c r="AJ1" s="661" t="s">
+      <c r="AI1" s="682"/>
+      <c r="AJ1" s="686" t="s">
         <v>575</v>
       </c>
-      <c r="AK1" s="661"/>
-      <c r="AL1" s="690" t="s">
+      <c r="AK1" s="686"/>
+      <c r="AL1" s="695" t="s">
         <v>576</v>
       </c>
-      <c r="AM1" s="691"/>
-      <c r="AN1" s="673" t="s">
+      <c r="AM1" s="696"/>
+      <c r="AN1" s="681" t="s">
         <v>577</v>
       </c>
-      <c r="AO1" s="674"/>
-      <c r="AP1" s="661" t="s">
+      <c r="AO1" s="682"/>
+      <c r="AP1" s="686" t="s">
         <v>578</v>
       </c>
-      <c r="AQ1" s="661"/>
-      <c r="AR1" s="690" t="s">
+      <c r="AQ1" s="686"/>
+      <c r="AR1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="AS1" s="691"/>
-      <c r="AT1" s="673" t="s">
+      <c r="AS1" s="696"/>
+      <c r="AT1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="AU1" s="674"/>
-      <c r="AV1" s="661" t="s">
+      <c r="AU1" s="682"/>
+      <c r="AV1" s="686" t="s">
         <v>579</v>
       </c>
-      <c r="AW1" s="661"/>
-      <c r="AX1" s="690" t="s">
+      <c r="AW1" s="686"/>
+      <c r="AX1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="AY1" s="691"/>
-      <c r="AZ1" s="673" t="s">
+      <c r="AY1" s="696"/>
+      <c r="AZ1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="BA1" s="674"/>
-      <c r="BB1" s="661" t="s">
+      <c r="BA1" s="682"/>
+      <c r="BB1" s="686" t="s">
         <v>580</v>
       </c>
-      <c r="BC1" s="661"/>
-      <c r="BD1" s="690" t="s">
+      <c r="BC1" s="686"/>
+      <c r="BD1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="BE1" s="691"/>
-      <c r="BF1" s="673" t="s">
+      <c r="BE1" s="696"/>
+      <c r="BF1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="BG1" s="674"/>
-      <c r="BH1" s="661" t="s">
+      <c r="BG1" s="682"/>
+      <c r="BH1" s="686" t="s">
         <v>581</v>
       </c>
-      <c r="BI1" s="661"/>
-      <c r="BJ1" s="690" t="s">
+      <c r="BI1" s="686"/>
+      <c r="BJ1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="BK1" s="691"/>
-      <c r="BL1" s="673" t="s">
+      <c r="BK1" s="696"/>
+      <c r="BL1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="BM1" s="674"/>
-      <c r="BN1" s="661" t="s">
+      <c r="BM1" s="682"/>
+      <c r="BN1" s="686" t="s">
         <v>582</v>
       </c>
-      <c r="BO1" s="661"/>
-      <c r="BP1" s="690" t="s">
+      <c r="BO1" s="686"/>
+      <c r="BP1" s="695" t="s">
         <v>570</v>
       </c>
-      <c r="BQ1" s="691"/>
-      <c r="BR1" s="673" t="s">
+      <c r="BQ1" s="696"/>
+      <c r="BR1" s="681" t="s">
         <v>568</v>
       </c>
-      <c r="BS1" s="674"/>
-      <c r="BT1" s="661" t="s">
+      <c r="BS1" s="682"/>
+      <c r="BT1" s="686" t="s">
         <v>583</v>
       </c>
-      <c r="BU1" s="661"/>
-      <c r="BV1" s="690" t="s">
+      <c r="BU1" s="686"/>
+      <c r="BV1" s="695" t="s">
         <v>584</v>
       </c>
-      <c r="BW1" s="691"/>
-      <c r="BX1" s="673" t="s">
+      <c r="BW1" s="696"/>
+      <c r="BX1" s="681" t="s">
         <v>585</v>
       </c>
-      <c r="BY1" s="674"/>
-      <c r="BZ1" s="661" t="s">
+      <c r="BY1" s="682"/>
+      <c r="BZ1" s="686" t="s">
         <v>586</v>
       </c>
-      <c r="CA1" s="661"/>
-      <c r="CB1" s="690" t="s">
+      <c r="CA1" s="686"/>
+      <c r="CB1" s="695" t="s">
         <v>587</v>
       </c>
-      <c r="CC1" s="691"/>
-      <c r="CD1" s="673" t="s">
+      <c r="CC1" s="696"/>
+      <c r="CD1" s="681" t="s">
         <v>588</v>
       </c>
-      <c r="CE1" s="674"/>
-      <c r="CF1" s="661" t="s">
+      <c r="CE1" s="682"/>
+      <c r="CF1" s="686" t="s">
         <v>589</v>
       </c>
-      <c r="CG1" s="661"/>
-      <c r="CH1" s="690" t="s">
+      <c r="CG1" s="686"/>
+      <c r="CH1" s="695" t="s">
         <v>587</v>
       </c>
-      <c r="CI1" s="691"/>
-      <c r="CJ1" s="673" t="s">
+      <c r="CI1" s="696"/>
+      <c r="CJ1" s="681" t="s">
         <v>588</v>
       </c>
-      <c r="CK1" s="674"/>
-      <c r="CL1" s="661" t="s">
+      <c r="CK1" s="682"/>
+      <c r="CL1" s="686" t="s">
         <v>590</v>
       </c>
-      <c r="CM1" s="661"/>
-      <c r="CN1" s="690" t="s">
+      <c r="CM1" s="686"/>
+      <c r="CN1" s="695" t="s">
         <v>587</v>
       </c>
-      <c r="CO1" s="691"/>
-      <c r="CP1" s="673" t="s">
+      <c r="CO1" s="696"/>
+      <c r="CP1" s="681" t="s">
         <v>588</v>
       </c>
-      <c r="CQ1" s="674"/>
-      <c r="CR1" s="661" t="s">
+      <c r="CQ1" s="682"/>
+      <c r="CR1" s="686" t="s">
         <v>591</v>
       </c>
-      <c r="CS1" s="661"/>
-      <c r="CT1" s="690" t="s">
+      <c r="CS1" s="686"/>
+      <c r="CT1" s="695" t="s">
         <v>587</v>
       </c>
-      <c r="CU1" s="691"/>
-      <c r="CV1" s="692" t="s">
+      <c r="CU1" s="696"/>
+      <c r="CV1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="CW1" s="693"/>
-      <c r="CX1" s="661" t="s">
+      <c r="CW1" s="698"/>
+      <c r="CX1" s="686" t="s">
         <v>592</v>
       </c>
-      <c r="CY1" s="661"/>
-      <c r="CZ1" s="690" t="s">
+      <c r="CY1" s="686"/>
+      <c r="CZ1" s="695" t="s">
         <v>587</v>
       </c>
-      <c r="DA1" s="691"/>
-      <c r="DB1" s="692" t="s">
+      <c r="DA1" s="696"/>
+      <c r="DB1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="DC1" s="693"/>
-      <c r="DD1" s="661" t="s">
+      <c r="DC1" s="698"/>
+      <c r="DD1" s="686" t="s">
         <v>593</v>
       </c>
-      <c r="DE1" s="661"/>
-      <c r="DF1" s="690" t="s">
+      <c r="DE1" s="686"/>
+      <c r="DF1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="DG1" s="691"/>
-      <c r="DH1" s="692" t="s">
+      <c r="DG1" s="696"/>
+      <c r="DH1" s="697" t="s">
         <v>595</v>
       </c>
-      <c r="DI1" s="693"/>
-      <c r="DJ1" s="661" t="s">
+      <c r="DI1" s="698"/>
+      <c r="DJ1" s="686" t="s">
         <v>596</v>
       </c>
-      <c r="DK1" s="661"/>
-      <c r="DL1" s="690" t="s">
+      <c r="DK1" s="686"/>
+      <c r="DL1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="DM1" s="691"/>
-      <c r="DN1" s="692" t="s">
+      <c r="DM1" s="696"/>
+      <c r="DN1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="DO1" s="693"/>
-      <c r="DP1" s="661" t="s">
+      <c r="DO1" s="698"/>
+      <c r="DP1" s="686" t="s">
         <v>597</v>
       </c>
-      <c r="DQ1" s="661"/>
-      <c r="DR1" s="690" t="s">
+      <c r="DQ1" s="686"/>
+      <c r="DR1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="DS1" s="691"/>
-      <c r="DT1" s="692" t="s">
+      <c r="DS1" s="696"/>
+      <c r="DT1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="DU1" s="693"/>
-      <c r="DV1" s="661" t="s">
+      <c r="DU1" s="698"/>
+      <c r="DV1" s="686" t="s">
         <v>598</v>
       </c>
-      <c r="DW1" s="661"/>
-      <c r="DX1" s="690" t="s">
+      <c r="DW1" s="686"/>
+      <c r="DX1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="DY1" s="691"/>
-      <c r="DZ1" s="692" t="s">
+      <c r="DY1" s="696"/>
+      <c r="DZ1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="EA1" s="693"/>
-      <c r="EB1" s="661" t="s">
+      <c r="EA1" s="698"/>
+      <c r="EB1" s="686" t="s">
         <v>599</v>
       </c>
-      <c r="EC1" s="661"/>
-      <c r="ED1" s="690" t="s">
+      <c r="EC1" s="686"/>
+      <c r="ED1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="EE1" s="691"/>
-      <c r="EF1" s="692" t="s">
+      <c r="EE1" s="696"/>
+      <c r="EF1" s="697" t="s">
         <v>588</v>
       </c>
-      <c r="EG1" s="693"/>
-      <c r="EH1" s="661" t="s">
+      <c r="EG1" s="698"/>
+      <c r="EH1" s="686" t="s">
         <v>600</v>
       </c>
-      <c r="EI1" s="661"/>
-      <c r="EJ1" s="690" t="s">
+      <c r="EI1" s="686"/>
+      <c r="EJ1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="EK1" s="691"/>
-      <c r="EL1" s="692" t="s">
+      <c r="EK1" s="696"/>
+      <c r="EL1" s="697" t="s">
         <v>601</v>
       </c>
-      <c r="EM1" s="693"/>
-      <c r="EN1" s="661" t="s">
+      <c r="EM1" s="698"/>
+      <c r="EN1" s="686" t="s">
         <v>602</v>
       </c>
-      <c r="EO1" s="661"/>
-      <c r="EP1" s="690" t="s">
+      <c r="EO1" s="686"/>
+      <c r="EP1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="EQ1" s="691"/>
-      <c r="ER1" s="692" t="s">
+      <c r="EQ1" s="696"/>
+      <c r="ER1" s="697" t="s">
         <v>603</v>
       </c>
-      <c r="ES1" s="693"/>
-      <c r="ET1" s="661" t="s">
+      <c r="ES1" s="698"/>
+      <c r="ET1" s="686" t="s">
         <v>604</v>
       </c>
-      <c r="EU1" s="661"/>
-      <c r="EV1" s="690" t="s">
+      <c r="EU1" s="686"/>
+      <c r="EV1" s="695" t="s">
         <v>594</v>
       </c>
-      <c r="EW1" s="691"/>
-      <c r="EX1" s="692" t="s">
+      <c r="EW1" s="696"/>
+      <c r="EX1" s="697" t="s">
         <v>103</v>
       </c>
-      <c r="EY1" s="693"/>
-      <c r="EZ1" s="661" t="s">
+      <c r="EY1" s="698"/>
+      <c r="EZ1" s="686" t="s">
         <v>605</v>
       </c>
-      <c r="FA1" s="661"/>
+      <c r="FA1" s="686"/>
       <c r="FC1" s="28" t="s">
         <v>606</v>
       </c>
@@ -27109,7 +27112,7 @@
       <c r="CT7" s="694" t="s">
         <v>672</v>
       </c>
-      <c r="CU7" s="661"/>
+      <c r="CU7" s="686"/>
       <c r="CV7" s="66" t="s">
         <v>670</v>
       </c>
@@ -27592,7 +27595,7 @@
       <c r="CZ8" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="DA8" s="661"/>
+      <c r="DA8" s="686"/>
       <c r="DB8" s="14" t="s">
         <v>700</v>
       </c>
@@ -27609,7 +27612,7 @@
       <c r="DF8" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="DG8" s="661"/>
+      <c r="DG8" s="686"/>
       <c r="DH8" s="14" t="s">
         <v>700</v>
       </c>
@@ -27626,7 +27629,7 @@
       <c r="DL8" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="DM8" s="661"/>
+      <c r="DM8" s="686"/>
       <c r="DN8" s="14" t="s">
         <v>700</v>
       </c>
@@ -27643,7 +27646,7 @@
       <c r="DR8" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="DS8" s="661"/>
+      <c r="DS8" s="686"/>
       <c r="DT8" s="14" t="s">
         <v>700</v>
       </c>
@@ -27656,7 +27659,7 @@
       <c r="DX8" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="DY8" s="661"/>
+      <c r="DY8" s="686"/>
       <c r="DZ8" s="14" t="s">
         <v>700</v>
       </c>
@@ -27693,7 +27696,7 @@
       <c r="EJ8" s="694" t="s">
         <v>703</v>
       </c>
-      <c r="EK8" s="661"/>
+      <c r="EK8" s="686"/>
       <c r="EL8" s="14" t="s">
         <v>700</v>
       </c>
@@ -28107,7 +28110,7 @@
       <c r="EP9" s="694" t="s">
         <v>703</v>
       </c>
-      <c r="EQ9" s="661"/>
+      <c r="EQ9" s="686"/>
       <c r="ER9" s="14" t="s">
         <v>718</v>
       </c>
@@ -28124,7 +28127,7 @@
       <c r="EV9" s="694" t="s">
         <v>703</v>
       </c>
-      <c r="EW9" s="661"/>
+      <c r="EW9" s="686"/>
       <c r="EX9" s="14" t="s">
         <v>718</v>
       </c>
@@ -28670,7 +28673,7 @@
       <c r="ED11" s="694" t="s">
         <v>703</v>
       </c>
-      <c r="EE11" s="661"/>
+      <c r="EE11" s="686"/>
       <c r="EF11" s="14" t="s">
         <v>760</v>
       </c>
@@ -28919,7 +28922,7 @@
       <c r="CT12" s="694" t="s">
         <v>702</v>
       </c>
-      <c r="CU12" s="661"/>
+      <c r="CU12" s="686"/>
       <c r="CX12" s="9" t="s">
         <v>696</v>
       </c>
@@ -30476,10 +30479,10 @@
       <c r="CQ19">
         <v>23</v>
       </c>
-      <c r="CT19" s="668" t="s">
+      <c r="CT19" s="669" t="s">
         <v>912</v>
       </c>
-      <c r="CU19" s="668"/>
+      <c r="CU19" s="669"/>
       <c r="CX19" t="s">
         <v>913</v>
       </c>
@@ -30782,20 +30785,20 @@
       <c r="EY21" s="14">
         <v>3</v>
       </c>
-      <c r="EZ21" s="697" t="s">
+      <c r="EZ21" s="692" t="s">
         <v>943</v>
       </c>
-      <c r="FA21" s="697"/>
+      <c r="FA21" s="692"/>
       <c r="FC21" s="366">
         <f>FC20-FC22</f>
         <v>113457.16899999997</v>
       </c>
       <c r="FD21" s="344"/>
-      <c r="FE21" s="698" t="s">
+      <c r="FE21" s="693" t="s">
         <v>945</v>
       </c>
-      <c r="FF21" s="698"/>
-      <c r="FG21" s="698"/>
+      <c r="FF21" s="693"/>
+      <c r="FG21" s="693"/>
     </row>
     <row r="22" spans="12:163">
       <c r="AH22" t="s">
@@ -30880,10 +30883,10 @@
       <c r="ET22" t="s">
         <v>953</v>
       </c>
-      <c r="EZ22" s="697" t="s">
+      <c r="EZ22" s="692" t="s">
         <v>953</v>
       </c>
-      <c r="FA22" s="697"/>
+      <c r="FA22" s="692"/>
       <c r="FC22" s="365">
         <f>E2+K2+Q2+W2+AC2+AI2+AO2+AU2+BA2+BG2+BM2+BS2+BY2+CE2+CK2+CQ2+CW2+DC2+DI2+DO2+DU2+EA2+EG2+EM2+ES2+EY2</f>
         <v>229252.68300000005</v>
@@ -31007,10 +31010,10 @@
       <c r="ET23" t="s">
         <v>966</v>
       </c>
-      <c r="EZ23" s="697" t="s">
+      <c r="EZ23" s="692" t="s">
         <v>969</v>
       </c>
-      <c r="FA23" s="697"/>
+      <c r="FA23" s="692"/>
       <c r="FC23" s="9" t="s">
         <v>970</v>
       </c>
@@ -31084,10 +31087,10 @@
         <v>978</v>
       </c>
       <c r="EY24" s="66"/>
-      <c r="EZ24" s="697" t="s">
+      <c r="EZ24" s="692" t="s">
         <v>979</v>
       </c>
-      <c r="FA24" s="697"/>
+      <c r="FA24" s="692"/>
       <c r="FC24" s="367">
         <f>SUM(FD25:FD26)</f>
         <v>178477.61000000002</v>
@@ -31255,7 +31258,7 @@
       </c>
       <c r="ER29" s="357"/>
       <c r="EX29" s="357"/>
-      <c r="FC29" s="695" t="s">
+      <c r="FC29" s="690" t="s">
         <v>998</v>
       </c>
       <c r="FD29" s="368">
@@ -31275,7 +31278,7 @@
       </c>
       <c r="ED30" s="357"/>
       <c r="EL30" s="357"/>
-      <c r="FC30" s="696"/>
+      <c r="FC30" s="691"/>
       <c r="FD30" s="368">
         <f>300*28+0.01</f>
         <v>8400.01</v>
@@ -31302,7 +31305,7 @@
       <c r="DQ31" s="357"/>
       <c r="DR31" s="357"/>
       <c r="DX31" s="357"/>
-      <c r="FC31" s="695" t="s">
+      <c r="FC31" s="690" t="s">
         <v>1003</v>
       </c>
       <c r="FD31" s="368">
@@ -31324,7 +31327,7 @@
       <c r="BY32">
         <v>9</v>
       </c>
-      <c r="FC32" s="696"/>
+      <c r="FC32" s="691"/>
       <c r="FD32" s="372">
         <f>FC22-FC24-SUM(FD29:FD31)</f>
         <v>11389.822000000036</v>
@@ -31459,18 +31462,75 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="FC29:FC30"/>
-    <mergeCell ref="FC31:FC32"/>
-    <mergeCell ref="EZ21:FA21"/>
-    <mergeCell ref="FE21:FG21"/>
-    <mergeCell ref="EZ22:FA22"/>
-    <mergeCell ref="EZ23:FA23"/>
-    <mergeCell ref="EZ24:FA24"/>
-    <mergeCell ref="EP9:EQ9"/>
-    <mergeCell ref="EV9:EW9"/>
-    <mergeCell ref="ED11:EE11"/>
-    <mergeCell ref="CT12:CU12"/>
-    <mergeCell ref="CT19:CU19"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BH1:BI1"/>
+    <mergeCell ref="BJ1:BK1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="BN1:BO1"/>
+    <mergeCell ref="BP1:BQ1"/>
+    <mergeCell ref="BR1:BS1"/>
+    <mergeCell ref="BT1:BU1"/>
+    <mergeCell ref="BV1:BW1"/>
+    <mergeCell ref="BX1:BY1"/>
+    <mergeCell ref="BZ1:CA1"/>
+    <mergeCell ref="CB1:CC1"/>
+    <mergeCell ref="CD1:CE1"/>
+    <mergeCell ref="CF1:CG1"/>
+    <mergeCell ref="CH1:CI1"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="CL1:CM1"/>
+    <mergeCell ref="CN1:CO1"/>
+    <mergeCell ref="CP1:CQ1"/>
+    <mergeCell ref="CR1:CS1"/>
+    <mergeCell ref="CT1:CU1"/>
+    <mergeCell ref="CV1:CW1"/>
+    <mergeCell ref="CX1:CY1"/>
+    <mergeCell ref="CZ1:DA1"/>
+    <mergeCell ref="DB1:DC1"/>
+    <mergeCell ref="DD1:DE1"/>
+    <mergeCell ref="DF1:DG1"/>
+    <mergeCell ref="DH1:DI1"/>
+    <mergeCell ref="DJ1:DK1"/>
+    <mergeCell ref="DL1:DM1"/>
+    <mergeCell ref="DN1:DO1"/>
+    <mergeCell ref="DP1:DQ1"/>
+    <mergeCell ref="ED1:EE1"/>
+    <mergeCell ref="EF1:EG1"/>
+    <mergeCell ref="EH1:EI1"/>
+    <mergeCell ref="EJ1:EK1"/>
+    <mergeCell ref="DR1:DS1"/>
+    <mergeCell ref="DT1:DU1"/>
+    <mergeCell ref="DV1:DW1"/>
+    <mergeCell ref="DX1:DY1"/>
+    <mergeCell ref="DZ1:EA1"/>
     <mergeCell ref="EV1:EW1"/>
     <mergeCell ref="EX1:EY1"/>
     <mergeCell ref="EZ1:FA1"/>
@@ -31487,75 +31547,18 @@
     <mergeCell ref="ER1:ES1"/>
     <mergeCell ref="ET1:EU1"/>
     <mergeCell ref="EB1:EC1"/>
-    <mergeCell ref="ED1:EE1"/>
-    <mergeCell ref="EF1:EG1"/>
-    <mergeCell ref="EH1:EI1"/>
-    <mergeCell ref="EJ1:EK1"/>
-    <mergeCell ref="DR1:DS1"/>
-    <mergeCell ref="DT1:DU1"/>
-    <mergeCell ref="DV1:DW1"/>
-    <mergeCell ref="DX1:DY1"/>
-    <mergeCell ref="DZ1:EA1"/>
-    <mergeCell ref="DH1:DI1"/>
-    <mergeCell ref="DJ1:DK1"/>
-    <mergeCell ref="DL1:DM1"/>
-    <mergeCell ref="DN1:DO1"/>
-    <mergeCell ref="DP1:DQ1"/>
-    <mergeCell ref="CX1:CY1"/>
-    <mergeCell ref="CZ1:DA1"/>
-    <mergeCell ref="DB1:DC1"/>
-    <mergeCell ref="DD1:DE1"/>
-    <mergeCell ref="DF1:DG1"/>
-    <mergeCell ref="CN1:CO1"/>
-    <mergeCell ref="CP1:CQ1"/>
-    <mergeCell ref="CR1:CS1"/>
-    <mergeCell ref="CT1:CU1"/>
-    <mergeCell ref="CV1:CW1"/>
-    <mergeCell ref="CD1:CE1"/>
-    <mergeCell ref="CF1:CG1"/>
-    <mergeCell ref="CH1:CI1"/>
-    <mergeCell ref="CJ1:CK1"/>
-    <mergeCell ref="CL1:CM1"/>
-    <mergeCell ref="BT1:BU1"/>
-    <mergeCell ref="BV1:BW1"/>
-    <mergeCell ref="BX1:BY1"/>
-    <mergeCell ref="BZ1:CA1"/>
-    <mergeCell ref="CB1:CC1"/>
-    <mergeCell ref="BJ1:BK1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="BN1:BO1"/>
-    <mergeCell ref="BP1:BQ1"/>
-    <mergeCell ref="BR1:BS1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BH1:BI1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="EP9:EQ9"/>
+    <mergeCell ref="EV9:EW9"/>
+    <mergeCell ref="ED11:EE11"/>
+    <mergeCell ref="CT12:CU12"/>
+    <mergeCell ref="CT19:CU19"/>
+    <mergeCell ref="FC29:FC30"/>
+    <mergeCell ref="FC31:FC32"/>
+    <mergeCell ref="EZ21:FA21"/>
+    <mergeCell ref="FE21:FG21"/>
+    <mergeCell ref="EZ22:FA22"/>
+    <mergeCell ref="EZ23:FA23"/>
+    <mergeCell ref="EZ24:FA24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -31770,7 +31773,7 @@
   <dimension ref="A1:NH79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="MU1" workbookViewId="0">
-      <selection activeCell="ND24" sqref="ND24"/>
+      <selection activeCell="NC21" sqref="NC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75"/>
@@ -32149,547 +32152,547 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:372">
-      <c r="A1" s="706" t="s">
+      <c r="A1" s="703" t="s">
         <v>1017</v>
       </c>
-      <c r="B1" s="706"/>
-      <c r="C1" s="675" t="s">
+      <c r="B1" s="703"/>
+      <c r="C1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="676"/>
-      <c r="E1" s="677" t="s">
+      <c r="D1" s="678"/>
+      <c r="E1" s="667" t="s">
         <v>1018</v>
       </c>
-      <c r="F1" s="678"/>
-      <c r="G1" s="706" t="s">
+      <c r="F1" s="668"/>
+      <c r="G1" s="703" t="s">
         <v>1019</v>
       </c>
-      <c r="H1" s="706"/>
-      <c r="I1" s="675" t="s">
+      <c r="H1" s="703"/>
+      <c r="I1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="676"/>
-      <c r="K1" s="677" t="s">
+      <c r="J1" s="678"/>
+      <c r="K1" s="667" t="s">
         <v>1020</v>
       </c>
-      <c r="L1" s="678"/>
-      <c r="M1" s="706" t="s">
+      <c r="L1" s="668"/>
+      <c r="M1" s="703" t="s">
         <v>1021</v>
       </c>
-      <c r="N1" s="706"/>
-      <c r="O1" s="675" t="s">
+      <c r="N1" s="703"/>
+      <c r="O1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="676"/>
-      <c r="Q1" s="677" t="s">
+      <c r="P1" s="678"/>
+      <c r="Q1" s="667" t="s">
         <v>1022</v>
       </c>
-      <c r="R1" s="678"/>
-      <c r="S1" s="706" t="s">
+      <c r="R1" s="668"/>
+      <c r="S1" s="703" t="s">
         <v>1023</v>
       </c>
-      <c r="T1" s="706"/>
-      <c r="U1" s="675" t="s">
+      <c r="T1" s="703"/>
+      <c r="U1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="676"/>
-      <c r="W1" s="677" t="s">
+      <c r="V1" s="678"/>
+      <c r="W1" s="667" t="s">
         <v>577</v>
       </c>
-      <c r="X1" s="678"/>
-      <c r="Y1" s="706" t="s">
+      <c r="X1" s="668"/>
+      <c r="Y1" s="703" t="s">
         <v>1024</v>
       </c>
-      <c r="Z1" s="706"/>
-      <c r="AA1" s="675" t="s">
+      <c r="Z1" s="703"/>
+      <c r="AA1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="AB1" s="676"/>
-      <c r="AC1" s="677" t="s">
+      <c r="AB1" s="678"/>
+      <c r="AC1" s="667" t="s">
         <v>1025</v>
       </c>
-      <c r="AD1" s="678"/>
-      <c r="AE1" s="706" t="s">
+      <c r="AD1" s="668"/>
+      <c r="AE1" s="703" t="s">
         <v>1026</v>
       </c>
-      <c r="AF1" s="706"/>
-      <c r="AG1" s="675" t="s">
+      <c r="AF1" s="703"/>
+      <c r="AG1" s="677" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" s="676"/>
-      <c r="AI1" s="677" t="s">
+      <c r="AH1" s="678"/>
+      <c r="AI1" s="667" t="s">
         <v>1027</v>
       </c>
-      <c r="AJ1" s="678"/>
-      <c r="AK1" s="706" t="s">
+      <c r="AJ1" s="668"/>
+      <c r="AK1" s="703" t="s">
         <v>1028</v>
       </c>
-      <c r="AL1" s="706"/>
-      <c r="AM1" s="675" t="s">
+      <c r="AL1" s="703"/>
+      <c r="AM1" s="677" t="s">
         <v>1029</v>
       </c>
-      <c r="AN1" s="676"/>
-      <c r="AO1" s="677" t="s">
+      <c r="AN1" s="678"/>
+      <c r="AO1" s="667" t="s">
         <v>1030</v>
       </c>
-      <c r="AP1" s="678"/>
-      <c r="AQ1" s="706" t="s">
+      <c r="AP1" s="668"/>
+      <c r="AQ1" s="703" t="s">
         <v>1031</v>
       </c>
-      <c r="AR1" s="706"/>
-      <c r="AS1" s="675" t="s">
+      <c r="AR1" s="703"/>
+      <c r="AS1" s="677" t="s">
         <v>1029</v>
       </c>
-      <c r="AT1" s="676"/>
-      <c r="AU1" s="677" t="s">
+      <c r="AT1" s="678"/>
+      <c r="AU1" s="667" t="s">
         <v>1032</v>
       </c>
-      <c r="AV1" s="678"/>
-      <c r="AW1" s="706" t="s">
+      <c r="AV1" s="668"/>
+      <c r="AW1" s="703" t="s">
         <v>1033</v>
       </c>
-      <c r="AX1" s="706"/>
-      <c r="AY1" s="677" t="s">
+      <c r="AX1" s="703"/>
+      <c r="AY1" s="667" t="s">
         <v>1034</v>
       </c>
-      <c r="AZ1" s="678"/>
-      <c r="BA1" s="706" t="s">
+      <c r="AZ1" s="668"/>
+      <c r="BA1" s="703" t="s">
         <v>1033</v>
       </c>
-      <c r="BB1" s="706"/>
-      <c r="BC1" s="675" t="s">
+      <c r="BB1" s="703"/>
+      <c r="BC1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="BD1" s="676"/>
-      <c r="BE1" s="677" t="s">
+      <c r="BD1" s="678"/>
+      <c r="BE1" s="667" t="s">
         <v>1035</v>
       </c>
-      <c r="BF1" s="678"/>
-      <c r="BG1" s="706" t="s">
+      <c r="BF1" s="668"/>
+      <c r="BG1" s="703" t="s">
         <v>1036</v>
       </c>
-      <c r="BH1" s="706"/>
-      <c r="BI1" s="675" t="s">
+      <c r="BH1" s="703"/>
+      <c r="BI1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="BJ1" s="676"/>
-      <c r="BK1" s="677" t="s">
+      <c r="BJ1" s="678"/>
+      <c r="BK1" s="667" t="s">
         <v>1035</v>
       </c>
-      <c r="BL1" s="678"/>
-      <c r="BM1" s="706" t="s">
+      <c r="BL1" s="668"/>
+      <c r="BM1" s="703" t="s">
         <v>1037</v>
       </c>
-      <c r="BN1" s="706"/>
-      <c r="BO1" s="675" t="s">
+      <c r="BN1" s="703"/>
+      <c r="BO1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="BP1" s="676"/>
-      <c r="BQ1" s="677" t="s">
+      <c r="BP1" s="678"/>
+      <c r="BQ1" s="667" t="s">
         <v>1038</v>
       </c>
-      <c r="BR1" s="678"/>
-      <c r="BS1" s="706" t="s">
+      <c r="BR1" s="668"/>
+      <c r="BS1" s="703" t="s">
         <v>1039</v>
       </c>
-      <c r="BT1" s="706"/>
-      <c r="BU1" s="675" t="s">
+      <c r="BT1" s="703"/>
+      <c r="BU1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="BV1" s="676"/>
-      <c r="BW1" s="677" t="s">
+      <c r="BV1" s="678"/>
+      <c r="BW1" s="667" t="s">
         <v>1040</v>
       </c>
-      <c r="BX1" s="678"/>
-      <c r="BY1" s="706" t="s">
+      <c r="BX1" s="668"/>
+      <c r="BY1" s="703" t="s">
         <v>1041</v>
       </c>
-      <c r="BZ1" s="706"/>
-      <c r="CA1" s="675" t="s">
+      <c r="BZ1" s="703"/>
+      <c r="CA1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="CB1" s="676"/>
-      <c r="CC1" s="677" t="s">
+      <c r="CB1" s="678"/>
+      <c r="CC1" s="667" t="s">
         <v>1038</v>
       </c>
-      <c r="CD1" s="678"/>
-      <c r="CE1" s="706" t="s">
+      <c r="CD1" s="668"/>
+      <c r="CE1" s="703" t="s">
         <v>1042</v>
       </c>
-      <c r="CF1" s="706"/>
-      <c r="CG1" s="675" t="s">
+      <c r="CF1" s="703"/>
+      <c r="CG1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="CH1" s="676"/>
-      <c r="CI1" s="677" t="s">
+      <c r="CH1" s="678"/>
+      <c r="CI1" s="667" t="s">
         <v>1040</v>
       </c>
-      <c r="CJ1" s="678"/>
-      <c r="CK1" s="706" t="s">
+      <c r="CJ1" s="668"/>
+      <c r="CK1" s="703" t="s">
         <v>1043</v>
       </c>
-      <c r="CL1" s="706"/>
-      <c r="CM1" s="675" t="s">
+      <c r="CL1" s="703"/>
+      <c r="CM1" s="677" t="s">
         <v>594</v>
       </c>
-      <c r="CN1" s="676"/>
-      <c r="CO1" s="677" t="s">
+      <c r="CN1" s="678"/>
+      <c r="CO1" s="667" t="s">
         <v>1038</v>
       </c>
-      <c r="CP1" s="678"/>
-      <c r="CQ1" s="706" t="s">
+      <c r="CP1" s="668"/>
+      <c r="CQ1" s="703" t="s">
         <v>1044</v>
       </c>
-      <c r="CR1" s="706"/>
-      <c r="CS1" s="707" t="s">
+      <c r="CR1" s="703"/>
+      <c r="CS1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="CT1" s="708"/>
-      <c r="CU1" s="677" t="s">
+      <c r="CT1" s="725"/>
+      <c r="CU1" s="667" t="s">
         <v>1045</v>
       </c>
-      <c r="CV1" s="678"/>
-      <c r="CW1" s="706" t="s">
+      <c r="CV1" s="668"/>
+      <c r="CW1" s="703" t="s">
         <v>1046</v>
       </c>
-      <c r="CX1" s="706"/>
-      <c r="CY1" s="707" t="s">
+      <c r="CX1" s="703"/>
+      <c r="CY1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="CZ1" s="708"/>
-      <c r="DA1" s="677" t="s">
+      <c r="CZ1" s="725"/>
+      <c r="DA1" s="667" t="s">
         <v>1047</v>
       </c>
-      <c r="DB1" s="678"/>
-      <c r="DC1" s="706" t="s">
+      <c r="DB1" s="668"/>
+      <c r="DC1" s="703" t="s">
         <v>1048</v>
       </c>
-      <c r="DD1" s="706"/>
-      <c r="DE1" s="707" t="s">
+      <c r="DD1" s="703"/>
+      <c r="DE1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="DF1" s="708"/>
-      <c r="DG1" s="677" t="s">
+      <c r="DF1" s="725"/>
+      <c r="DG1" s="667" t="s">
         <v>1049</v>
       </c>
-      <c r="DH1" s="678"/>
-      <c r="DI1" s="706" t="s">
+      <c r="DH1" s="668"/>
+      <c r="DI1" s="703" t="s">
         <v>1050</v>
       </c>
-      <c r="DJ1" s="706"/>
-      <c r="DK1" s="707" t="s">
+      <c r="DJ1" s="703"/>
+      <c r="DK1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="DL1" s="708"/>
-      <c r="DM1" s="677" t="s">
+      <c r="DL1" s="725"/>
+      <c r="DM1" s="667" t="s">
         <v>1045</v>
       </c>
-      <c r="DN1" s="678"/>
-      <c r="DO1" s="706" t="s">
+      <c r="DN1" s="668"/>
+      <c r="DO1" s="703" t="s">
         <v>1051</v>
       </c>
-      <c r="DP1" s="706"/>
-      <c r="DQ1" s="707" t="s">
+      <c r="DP1" s="703"/>
+      <c r="DQ1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="DR1" s="708"/>
-      <c r="DS1" s="677" t="s">
+      <c r="DR1" s="725"/>
+      <c r="DS1" s="667" t="s">
         <v>1052</v>
       </c>
-      <c r="DT1" s="678"/>
-      <c r="DU1" s="706" t="s">
+      <c r="DT1" s="668"/>
+      <c r="DU1" s="703" t="s">
         <v>1053</v>
       </c>
-      <c r="DV1" s="706"/>
-      <c r="DW1" s="707" t="s">
+      <c r="DV1" s="703"/>
+      <c r="DW1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="DX1" s="708"/>
-      <c r="DY1" s="677" t="s">
+      <c r="DX1" s="725"/>
+      <c r="DY1" s="667" t="s">
         <v>1054</v>
       </c>
-      <c r="DZ1" s="678"/>
-      <c r="EA1" s="699" t="s">
+      <c r="DZ1" s="668"/>
+      <c r="EA1" s="719" t="s">
         <v>1055</v>
       </c>
-      <c r="EB1" s="699"/>
-      <c r="EC1" s="707" t="s">
+      <c r="EB1" s="719"/>
+      <c r="EC1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="ED1" s="708"/>
-      <c r="EE1" s="677" t="s">
+      <c r="ED1" s="725"/>
+      <c r="EE1" s="667" t="s">
         <v>1052</v>
       </c>
-      <c r="EF1" s="678"/>
+      <c r="EF1" s="668"/>
       <c r="EG1" s="53"/>
-      <c r="EH1" s="699" t="s">
+      <c r="EH1" s="719" t="s">
         <v>1056</v>
       </c>
-      <c r="EI1" s="699"/>
-      <c r="EJ1" s="707" t="s">
+      <c r="EI1" s="719"/>
+      <c r="EJ1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="EK1" s="708"/>
-      <c r="EL1" s="677" t="s">
+      <c r="EK1" s="725"/>
+      <c r="EL1" s="667" t="s">
         <v>1057</v>
       </c>
-      <c r="EM1" s="678"/>
-      <c r="EN1" s="699" t="s">
+      <c r="EM1" s="668"/>
+      <c r="EN1" s="719" t="s">
         <v>1058</v>
       </c>
-      <c r="EO1" s="699"/>
-      <c r="EP1" s="707" t="s">
+      <c r="EO1" s="719"/>
+      <c r="EP1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="EQ1" s="708"/>
-      <c r="ER1" s="677" t="s">
+      <c r="EQ1" s="725"/>
+      <c r="ER1" s="667" t="s">
         <v>1059</v>
       </c>
-      <c r="ES1" s="678"/>
-      <c r="ET1" s="699" t="s">
+      <c r="ES1" s="668"/>
+      <c r="ET1" s="719" t="s">
         <v>1060</v>
       </c>
-      <c r="EU1" s="699"/>
-      <c r="EV1" s="707" t="s">
+      <c r="EU1" s="719"/>
+      <c r="EV1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="EW1" s="708"/>
-      <c r="EX1" s="677" t="s">
+      <c r="EW1" s="725"/>
+      <c r="EX1" s="667" t="s">
         <v>1054</v>
       </c>
-      <c r="EY1" s="678"/>
-      <c r="EZ1" s="699" t="s">
+      <c r="EY1" s="668"/>
+      <c r="EZ1" s="719" t="s">
         <v>1061</v>
       </c>
-      <c r="FA1" s="699"/>
-      <c r="FB1" s="707" t="s">
+      <c r="FA1" s="719"/>
+      <c r="FB1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="FC1" s="708"/>
-      <c r="FD1" s="677" t="s">
+      <c r="FC1" s="725"/>
+      <c r="FD1" s="667" t="s">
         <v>1047</v>
       </c>
-      <c r="FE1" s="678"/>
-      <c r="FF1" s="699" t="s">
+      <c r="FE1" s="668"/>
+      <c r="FF1" s="719" t="s">
         <v>1062</v>
       </c>
-      <c r="FG1" s="699"/>
-      <c r="FH1" s="707" t="s">
+      <c r="FG1" s="719"/>
+      <c r="FH1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="FI1" s="708"/>
-      <c r="FJ1" s="677" t="s">
+      <c r="FI1" s="725"/>
+      <c r="FJ1" s="667" t="s">
         <v>1045</v>
       </c>
-      <c r="FK1" s="678"/>
-      <c r="FL1" s="699" t="s">
+      <c r="FK1" s="668"/>
+      <c r="FL1" s="719" t="s">
         <v>1063</v>
       </c>
-      <c r="FM1" s="699"/>
-      <c r="FN1" s="707" t="s">
+      <c r="FM1" s="719"/>
+      <c r="FN1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="FO1" s="708"/>
-      <c r="FP1" s="677" t="s">
+      <c r="FO1" s="725"/>
+      <c r="FP1" s="667" t="s">
         <v>1064</v>
       </c>
-      <c r="FQ1" s="678"/>
-      <c r="FR1" s="699" t="s">
+      <c r="FQ1" s="668"/>
+      <c r="FR1" s="719" t="s">
         <v>1065</v>
       </c>
-      <c r="FS1" s="699"/>
-      <c r="FT1" s="707" t="s">
+      <c r="FS1" s="719"/>
+      <c r="FT1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="FU1" s="708"/>
-      <c r="FV1" s="677" t="s">
+      <c r="FU1" s="725"/>
+      <c r="FV1" s="667" t="s">
         <v>1064</v>
       </c>
-      <c r="FW1" s="678"/>
-      <c r="FX1" s="699" t="s">
+      <c r="FW1" s="668"/>
+      <c r="FX1" s="719" t="s">
         <v>1066</v>
       </c>
-      <c r="FY1" s="699"/>
-      <c r="FZ1" s="707" t="s">
+      <c r="FY1" s="719"/>
+      <c r="FZ1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="GA1" s="708"/>
-      <c r="GB1" s="677" t="s">
+      <c r="GA1" s="725"/>
+      <c r="GB1" s="667" t="s">
         <v>1054</v>
       </c>
-      <c r="GC1" s="678"/>
-      <c r="GD1" s="699" t="s">
+      <c r="GC1" s="668"/>
+      <c r="GD1" s="719" t="s">
         <v>1067</v>
       </c>
-      <c r="GE1" s="699"/>
-      <c r="GF1" s="707" t="s">
+      <c r="GE1" s="719"/>
+      <c r="GF1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="GG1" s="708"/>
-      <c r="GH1" s="677" t="s">
+      <c r="GG1" s="725"/>
+      <c r="GH1" s="667" t="s">
         <v>1052</v>
       </c>
-      <c r="GI1" s="678"/>
-      <c r="GJ1" s="699" t="s">
+      <c r="GI1" s="668"/>
+      <c r="GJ1" s="719" t="s">
         <v>1068</v>
       </c>
-      <c r="GK1" s="699"/>
-      <c r="GL1" s="707" t="s">
+      <c r="GK1" s="719"/>
+      <c r="GL1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="GM1" s="708"/>
-      <c r="GN1" s="677" t="s">
+      <c r="GM1" s="725"/>
+      <c r="GN1" s="667" t="s">
         <v>1052</v>
       </c>
-      <c r="GO1" s="678"/>
-      <c r="GP1" s="699" t="s">
+      <c r="GO1" s="668"/>
+      <c r="GP1" s="719" t="s">
         <v>1069</v>
       </c>
-      <c r="GQ1" s="699"/>
-      <c r="GR1" s="707" t="s">
+      <c r="GQ1" s="719"/>
+      <c r="GR1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="GS1" s="708"/>
-      <c r="GT1" s="677" t="s">
+      <c r="GS1" s="725"/>
+      <c r="GT1" s="667" t="s">
         <v>1057</v>
       </c>
-      <c r="GU1" s="678"/>
-      <c r="GV1" s="699" t="s">
+      <c r="GU1" s="668"/>
+      <c r="GV1" s="719" t="s">
         <v>1070</v>
       </c>
-      <c r="GW1" s="699"/>
-      <c r="GX1" s="707" t="s">
+      <c r="GW1" s="719"/>
+      <c r="GX1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="GY1" s="708"/>
-      <c r="GZ1" s="677" t="s">
+      <c r="GY1" s="725"/>
+      <c r="GZ1" s="667" t="s">
         <v>1071</v>
       </c>
-      <c r="HA1" s="678"/>
-      <c r="HB1" s="699" t="s">
+      <c r="HA1" s="668"/>
+      <c r="HB1" s="719" t="s">
         <v>1072</v>
       </c>
-      <c r="HC1" s="699"/>
-      <c r="HD1" s="707" t="s">
+      <c r="HC1" s="719"/>
+      <c r="HD1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="HE1" s="708"/>
-      <c r="HF1" s="677" t="s">
+      <c r="HE1" s="725"/>
+      <c r="HF1" s="667" t="s">
         <v>1059</v>
       </c>
-      <c r="HG1" s="678"/>
-      <c r="HH1" s="699" t="s">
+      <c r="HG1" s="668"/>
+      <c r="HH1" s="719" t="s">
         <v>1073</v>
       </c>
-      <c r="HI1" s="699"/>
-      <c r="HJ1" s="707" t="s">
+      <c r="HI1" s="719"/>
+      <c r="HJ1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="HK1" s="708"/>
-      <c r="HL1" s="677" t="s">
+      <c r="HK1" s="725"/>
+      <c r="HL1" s="667" t="s">
         <v>1045</v>
       </c>
-      <c r="HM1" s="678"/>
-      <c r="HN1" s="699" t="s">
+      <c r="HM1" s="668"/>
+      <c r="HN1" s="719" t="s">
         <v>1074</v>
       </c>
-      <c r="HO1" s="699"/>
-      <c r="HP1" s="707" t="s">
+      <c r="HO1" s="719"/>
+      <c r="HP1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="HQ1" s="708"/>
-      <c r="HR1" s="677" t="s">
+      <c r="HQ1" s="725"/>
+      <c r="HR1" s="667" t="s">
         <v>1045</v>
       </c>
-      <c r="HS1" s="678"/>
-      <c r="HT1" s="699" t="s">
+      <c r="HS1" s="668"/>
+      <c r="HT1" s="719" t="s">
         <v>1075</v>
       </c>
-      <c r="HU1" s="699"/>
-      <c r="HV1" s="707" t="s">
+      <c r="HU1" s="719"/>
+      <c r="HV1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="HW1" s="708"/>
-      <c r="HX1" s="677" t="s">
+      <c r="HW1" s="725"/>
+      <c r="HX1" s="667" t="s">
         <v>1054</v>
       </c>
-      <c r="HY1" s="678"/>
-      <c r="HZ1" s="699" t="s">
+      <c r="HY1" s="668"/>
+      <c r="HZ1" s="719" t="s">
         <v>1076</v>
       </c>
-      <c r="IA1" s="699"/>
-      <c r="IB1" s="707" t="s">
+      <c r="IA1" s="719"/>
+      <c r="IB1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="IC1" s="708"/>
-      <c r="ID1" s="677" t="s">
+      <c r="IC1" s="725"/>
+      <c r="ID1" s="667" t="s">
         <v>1059</v>
       </c>
-      <c r="IE1" s="678"/>
-      <c r="IF1" s="699" t="s">
+      <c r="IE1" s="668"/>
+      <c r="IF1" s="719" t="s">
         <v>1077</v>
       </c>
-      <c r="IG1" s="699"/>
-      <c r="IH1" s="707" t="s">
+      <c r="IG1" s="719"/>
+      <c r="IH1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="II1" s="708"/>
-      <c r="IJ1" s="677" t="s">
+      <c r="II1" s="725"/>
+      <c r="IJ1" s="667" t="s">
         <v>1052</v>
       </c>
-      <c r="IK1" s="678"/>
-      <c r="IL1" s="699" t="s">
+      <c r="IK1" s="668"/>
+      <c r="IL1" s="719" t="s">
         <v>1078</v>
       </c>
-      <c r="IM1" s="699"/>
-      <c r="IN1" s="707" t="s">
+      <c r="IM1" s="719"/>
+      <c r="IN1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="IO1" s="708"/>
-      <c r="IP1" s="677" t="s">
+      <c r="IO1" s="725"/>
+      <c r="IP1" s="667" t="s">
         <v>1054</v>
       </c>
-      <c r="IQ1" s="678"/>
-      <c r="IR1" s="699" t="s">
+      <c r="IQ1" s="668"/>
+      <c r="IR1" s="719" t="s">
         <v>1079</v>
       </c>
-      <c r="IS1" s="699"/>
-      <c r="IT1" s="707" t="s">
+      <c r="IS1" s="719"/>
+      <c r="IT1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="IU1" s="708"/>
-      <c r="IV1" s="677" t="s">
+      <c r="IU1" s="725"/>
+      <c r="IV1" s="667" t="s">
         <v>1080</v>
       </c>
-      <c r="IW1" s="678"/>
-      <c r="IX1" s="699" t="s">
+      <c r="IW1" s="668"/>
+      <c r="IX1" s="719" t="s">
         <v>1081</v>
       </c>
-      <c r="IY1" s="699"/>
-      <c r="IZ1" s="707" t="s">
+      <c r="IY1" s="719"/>
+      <c r="IZ1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="JA1" s="708"/>
-      <c r="JB1" s="677" t="s">
+      <c r="JA1" s="725"/>
+      <c r="JB1" s="667" t="s">
         <v>1064</v>
       </c>
-      <c r="JC1" s="678"/>
-      <c r="JD1" s="699" t="s">
+      <c r="JC1" s="668"/>
+      <c r="JD1" s="719" t="s">
         <v>1082</v>
       </c>
-      <c r="JE1" s="699"/>
-      <c r="JF1" s="707" t="s">
+      <c r="JE1" s="719"/>
+      <c r="JF1" s="724" t="s">
         <v>594</v>
       </c>
-      <c r="JG1" s="708"/>
-      <c r="JH1" s="677" t="s">
+      <c r="JG1" s="725"/>
+      <c r="JH1" s="667" t="s">
         <v>1080</v>
       </c>
-      <c r="JI1" s="678"/>
-      <c r="JJ1" s="699" t="s">
+      <c r="JI1" s="668"/>
+      <c r="JJ1" s="719" t="s">
         <v>1083</v>
       </c>
-      <c r="JK1" s="699"/>
+      <c r="JK1" s="719"/>
       <c r="JL1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32698,10 +32701,10 @@
         <v>1080</v>
       </c>
       <c r="JO1" s="53"/>
-      <c r="JP1" s="699" t="s">
+      <c r="JP1" s="719" t="s">
         <v>1084</v>
       </c>
-      <c r="JQ1" s="699"/>
+      <c r="JQ1" s="719"/>
       <c r="JR1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32710,10 +32713,10 @@
         <v>1057</v>
       </c>
       <c r="JU1" s="53"/>
-      <c r="JV1" s="699" t="s">
+      <c r="JV1" s="719" t="s">
         <v>1085</v>
       </c>
-      <c r="JW1" s="699"/>
+      <c r="JW1" s="719"/>
       <c r="JX1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32722,10 +32725,10 @@
         <v>1086</v>
       </c>
       <c r="KA1" s="53"/>
-      <c r="KB1" s="699" t="s">
+      <c r="KB1" s="719" t="s">
         <v>1087</v>
       </c>
-      <c r="KC1" s="699"/>
+      <c r="KC1" s="719"/>
       <c r="KD1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32734,10 +32737,10 @@
         <v>1045</v>
       </c>
       <c r="KG1" s="53"/>
-      <c r="KH1" s="699" t="s">
+      <c r="KH1" s="719" t="s">
         <v>1088</v>
       </c>
-      <c r="KI1" s="699"/>
+      <c r="KI1" s="719"/>
       <c r="KJ1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32746,10 +32749,10 @@
         <v>1052</v>
       </c>
       <c r="KM1" s="53"/>
-      <c r="KN1" s="699" t="s">
+      <c r="KN1" s="719" t="s">
         <v>1089</v>
       </c>
-      <c r="KO1" s="699"/>
+      <c r="KO1" s="719"/>
       <c r="KP1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32758,10 +32761,10 @@
         <v>1052</v>
       </c>
       <c r="KS1" s="53"/>
-      <c r="KT1" s="699" t="s">
+      <c r="KT1" s="719" t="s">
         <v>1090</v>
       </c>
-      <c r="KU1" s="699"/>
+      <c r="KU1" s="719"/>
       <c r="KV1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32770,10 +32773,10 @@
         <v>1052</v>
       </c>
       <c r="KY1" s="53"/>
-      <c r="KZ1" s="699" t="s">
+      <c r="KZ1" s="719" t="s">
         <v>1091</v>
       </c>
-      <c r="LA1" s="699"/>
+      <c r="LA1" s="719"/>
       <c r="LB1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32782,10 +32785,10 @@
         <v>1080</v>
       </c>
       <c r="LE1" s="53"/>
-      <c r="LF1" s="699" t="s">
+      <c r="LF1" s="719" t="s">
         <v>1092</v>
       </c>
-      <c r="LG1" s="699"/>
+      <c r="LG1" s="719"/>
       <c r="LH1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32794,10 +32797,10 @@
         <v>1080</v>
       </c>
       <c r="LK1" s="53"/>
-      <c r="LL1" s="699" t="s">
+      <c r="LL1" s="719" t="s">
         <v>1093</v>
       </c>
-      <c r="LM1" s="699"/>
+      <c r="LM1" s="719"/>
       <c r="LN1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32806,10 +32809,10 @@
         <v>1080</v>
       </c>
       <c r="LQ1" s="53"/>
-      <c r="LR1" s="699" t="s">
+      <c r="LR1" s="719" t="s">
         <v>1094</v>
       </c>
-      <c r="LS1" s="699"/>
+      <c r="LS1" s="719"/>
       <c r="LT1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32818,10 +32821,10 @@
         <v>1064</v>
       </c>
       <c r="LW1" s="53"/>
-      <c r="LX1" s="699" t="s">
+      <c r="LX1" s="719" t="s">
         <v>1095</v>
       </c>
-      <c r="LY1" s="699"/>
+      <c r="LY1" s="719"/>
       <c r="LZ1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32830,10 +32833,10 @@
         <v>1080</v>
       </c>
       <c r="MC1" s="53"/>
-      <c r="MD1" s="709" t="s">
+      <c r="MD1" s="720" t="s">
         <v>1096</v>
       </c>
-      <c r="ME1" s="699"/>
+      <c r="ME1" s="719"/>
       <c r="MF1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32842,10 +32845,10 @@
         <v>1080</v>
       </c>
       <c r="MI1" s="53"/>
-      <c r="MJ1" s="709" t="s">
+      <c r="MJ1" s="720" t="s">
         <v>1097</v>
       </c>
-      <c r="MK1" s="699"/>
+      <c r="MK1" s="719"/>
       <c r="ML1" s="578" t="s">
         <v>594</v>
       </c>
@@ -32854,10 +32857,10 @@
         <v>1080</v>
       </c>
       <c r="MO1" s="53"/>
-      <c r="MP1" s="699" t="s">
+      <c r="MP1" s="719" t="s">
         <v>3427</v>
       </c>
-      <c r="MQ1" s="699"/>
+      <c r="MQ1" s="719"/>
       <c r="MR1" s="596" t="s">
         <v>594</v>
       </c>
@@ -32866,10 +32869,10 @@
         <v>1080</v>
       </c>
       <c r="MU1" s="594"/>
-      <c r="MV1" s="699" t="s">
+      <c r="MV1" s="719" t="s">
         <v>3484</v>
       </c>
-      <c r="MW1" s="699"/>
+      <c r="MW1" s="719"/>
       <c r="MX1" s="651" t="s">
         <v>594</v>
       </c>
@@ -32878,10 +32881,10 @@
         <v>1080</v>
       </c>
       <c r="NA1" s="649"/>
-      <c r="NB1" s="699" t="s">
+      <c r="NB1" s="719" t="s">
         <v>3490</v>
       </c>
-      <c r="NC1" s="699"/>
+      <c r="NC1" s="719"/>
     </row>
     <row r="2" spans="1:372">
       <c r="A2" s="54" t="s">
@@ -34076,10 +34079,10 @@
       </c>
     </row>
     <row r="3" spans="1:372">
-      <c r="A3" s="727" t="s">
+      <c r="A3" s="702" t="s">
         <v>1109</v>
       </c>
-      <c r="B3" s="727"/>
+      <c r="B3" s="702"/>
       <c r="E3" s="58" t="s">
         <v>123</v>
       </c>
@@ -34087,10 +34090,10 @@
         <f>F2-F4</f>
         <v>17</v>
       </c>
-      <c r="G3" s="727" t="s">
+      <c r="G3" s="702" t="s">
         <v>1109</v>
       </c>
-      <c r="H3" s="727"/>
+      <c r="H3" s="702"/>
       <c r="K3" s="58" t="s">
         <v>123</v>
       </c>
@@ -34924,12 +34927,12 @@
       </c>
       <c r="NC3" s="50">
         <f>SUM(NC13:NC14)</f>
-        <v>-176810</v>
+        <v>-63760</v>
       </c>
     </row>
     <row r="4" spans="1:372" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A4" s="727"/>
-      <c r="B4" s="727"/>
+      <c r="A4" s="702"/>
+      <c r="B4" s="702"/>
       <c r="E4" s="58" t="s">
         <v>134</v>
       </c>
@@ -34937,8 +34940,8 @@
         <f>SUM(F14:F57)</f>
         <v>12750</v>
       </c>
-      <c r="G4" s="727"/>
-      <c r="H4" s="727"/>
+      <c r="G4" s="702"/>
+      <c r="H4" s="702"/>
       <c r="K4" s="58" t="s">
         <v>134</v>
       </c>
@@ -44687,10 +44690,10 @@
       <c r="NF13" s="638" t="s">
         <v>3459</v>
       </c>
-      <c r="NG13" s="700" t="s">
+      <c r="NG13" s="726" t="s">
         <v>3462</v>
       </c>
-      <c r="NH13" s="704"/>
+      <c r="NH13" s="730"/>
     </row>
     <row r="14" spans="1:372">
       <c r="A14" s="21" t="s">
@@ -45000,10 +45003,10 @@
       <c r="DN14" s="62">
         <v>2700</v>
       </c>
-      <c r="DO14" s="710" t="s">
+      <c r="DO14" s="721" t="s">
         <v>1631</v>
       </c>
-      <c r="DP14" s="711"/>
+      <c r="DP14" s="722"/>
       <c r="DQ14" s="62" t="s">
         <v>1632</v>
       </c>
@@ -45247,10 +45250,10 @@
       <c r="HI14" s="14">
         <v>3063</v>
       </c>
-      <c r="HJ14" s="699" t="s">
+      <c r="HJ14" s="719" t="s">
         <v>1649</v>
       </c>
-      <c r="HK14" s="699"/>
+      <c r="HK14" s="719"/>
       <c r="HL14" s="169" t="s">
         <v>1547</v>
       </c>
@@ -45666,19 +45669,19 @@
       <c r="NB14" s="604" t="s">
         <v>3445</v>
       </c>
-      <c r="NC14" s="50">
-        <v>-113000</v>
+      <c r="NC14" s="586">
+        <v>50</v>
       </c>
       <c r="ND14" s="24">
-        <v>45503</v>
+        <v>45505</v>
       </c>
       <c r="NE14" s="154"/>
       <c r="NF14" s="639">
         <f>FLOOR(MW3,1000)</f>
         <v>-177000</v>
       </c>
-      <c r="NG14" s="701"/>
-      <c r="NH14" s="705"/>
+      <c r="NG14" s="727"/>
+      <c r="NH14" s="731"/>
     </row>
     <row r="15" spans="1:372">
       <c r="A15" s="21" t="s">
@@ -46388,10 +46391,10 @@
       <c r="KC15" s="50">
         <v>100491</v>
       </c>
-      <c r="KD15" s="712" t="s">
+      <c r="KD15" s="723" t="s">
         <v>1605</v>
       </c>
-      <c r="KE15" s="712"/>
+      <c r="KE15" s="723"/>
       <c r="KF15" s="169" t="s">
         <v>1723</v>
       </c>
@@ -47578,10 +47581,10 @@
         <v>45503</v>
       </c>
       <c r="NE16" s="154"/>
-      <c r="NF16" s="702" t="s">
+      <c r="NF16" s="728" t="s">
         <v>3458</v>
       </c>
-      <c r="NG16" s="703"/>
+      <c r="NG16" s="729"/>
       <c r="NH16" s="21"/>
     </row>
     <row r="17" spans="1:372" ht="12" customHeight="1">
@@ -48516,11 +48519,11 @@
       <c r="NB17" s="657" t="s">
         <v>1482</v>
       </c>
-      <c r="NC17" s="48">
-        <v>130917</v>
+      <c r="NC17" s="50">
+        <v>17867</v>
       </c>
       <c r="ND17" s="336" t="s">
-        <v>3512</v>
+        <v>3515</v>
       </c>
       <c r="NE17" s="636" t="s">
         <v>3464</v>
@@ -48771,10 +48774,10 @@
       <c r="DH18" s="62">
         <v>2000</v>
       </c>
-      <c r="DI18" s="710" t="s">
+      <c r="DI18" s="721" t="s">
         <v>1864</v>
       </c>
-      <c r="DJ18" s="711"/>
+      <c r="DJ18" s="722"/>
       <c r="DK18" s="62"/>
       <c r="DM18" s="119" t="s">
         <v>1560</v>
@@ -51345,17 +51348,17 @@
       <c r="L21" s="14">
         <v>0</v>
       </c>
-      <c r="M21" s="713" t="s">
+      <c r="M21" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="N21" s="713"/>
+      <c r="N21" s="718"/>
       <c r="Q21" s="63" t="s">
         <v>355</v>
       </c>
-      <c r="S21" s="713" t="s">
+      <c r="S21" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="T21" s="713"/>
+      <c r="T21" s="718"/>
       <c r="W21" s="71" t="s">
         <v>1680</v>
       </c>
@@ -51669,7 +51672,7 @@
       <c r="FB21" s="66" t="s">
         <v>2053</v>
       </c>
-      <c r="FC21" s="725" t="s">
+      <c r="FC21" s="700" t="s">
         <v>2054</v>
       </c>
       <c r="FD21" s="169" t="s">
@@ -52251,27 +52254,27 @@
       <c r="L22" s="14">
         <v>0</v>
       </c>
-      <c r="M22" s="715" t="s">
+      <c r="M22" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="N22" s="715"/>
+      <c r="N22" s="704"/>
       <c r="Q22" s="63" t="s">
         <v>364</v>
       </c>
-      <c r="S22" s="715" t="s">
+      <c r="S22" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="T22" s="715"/>
+      <c r="T22" s="704"/>
       <c r="W22" s="71" t="s">
         <v>1737</v>
       </c>
       <c r="X22" s="14">
         <v>0</v>
       </c>
-      <c r="Y22" s="713" t="s">
+      <c r="Y22" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="Z22" s="713"/>
+      <c r="Z22" s="718"/>
       <c r="AC22" s="72" t="s">
         <v>2093</v>
       </c>
@@ -52555,7 +52558,7 @@
         <v>2000</v>
       </c>
       <c r="FB22" s="66"/>
-      <c r="FC22" s="725"/>
+      <c r="FC22" s="700"/>
       <c r="FD22" s="169" t="s">
         <v>2049</v>
       </c>
@@ -52784,10 +52787,10 @@
       <c r="IR22" s="74" t="s">
         <v>2117</v>
       </c>
-      <c r="IT22" s="706" t="s">
+      <c r="IT22" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="IU22" s="706"/>
+      <c r="IU22" s="703"/>
       <c r="IV22" s="152" t="s">
         <v>2119</v>
       </c>
@@ -53097,49 +53100,49 @@
       </c>
     </row>
     <row r="23" spans="1:372">
-      <c r="A23" s="713" t="s">
+      <c r="A23" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="B23" s="713"/>
+      <c r="B23" s="718"/>
       <c r="E23" s="565" t="s">
         <v>402</v>
       </c>
       <c r="F23" s="63"/>
-      <c r="G23" s="713" t="s">
+      <c r="G23" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="H23" s="713"/>
+      <c r="H23" s="718"/>
       <c r="K23" s="71" t="s">
         <v>1737</v>
       </c>
       <c r="L23" s="14">
         <v>0</v>
       </c>
-      <c r="M23" s="714"/>
-      <c r="N23" s="714"/>
+      <c r="M23" s="710"/>
+      <c r="N23" s="710"/>
       <c r="Q23" s="63" t="s">
         <v>1917</v>
       </c>
-      <c r="S23" s="714"/>
-      <c r="T23" s="714"/>
+      <c r="S23" s="710"/>
+      <c r="T23" s="710"/>
       <c r="W23" s="71" t="s">
         <v>1518</v>
       </c>
       <c r="X23" s="66">
         <v>0</v>
       </c>
-      <c r="Y23" s="715" t="s">
+      <c r="Y23" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="Z23" s="715"/>
-      <c r="AE23" s="713" t="s">
+      <c r="Z23" s="704"/>
+      <c r="AE23" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="AF23" s="713"/>
-      <c r="AK23" s="713" t="s">
+      <c r="AF23" s="718"/>
+      <c r="AK23" s="718" t="s">
         <v>330</v>
       </c>
-      <c r="AL23" s="713"/>
+      <c r="AL23" s="718"/>
       <c r="AO23" s="71" t="s">
         <v>1617</v>
       </c>
@@ -53327,10 +53330,10 @@
       <c r="EB23" s="97">
         <v>5000</v>
       </c>
-      <c r="EE23" s="716" t="s">
+      <c r="EE23" s="715" t="s">
         <v>2150</v>
       </c>
-      <c r="EF23" s="716"/>
+      <c r="EF23" s="715"/>
       <c r="EH23" s="54" t="s">
         <v>1936</v>
       </c>
@@ -53366,7 +53369,7 @@
       <c r="EV23" s="66" t="s">
         <v>2151</v>
       </c>
-      <c r="EW23" s="725" t="s">
+      <c r="EW23" s="700" t="s">
         <v>2054</v>
       </c>
       <c r="EX23" s="152" t="s">
@@ -53383,7 +53386,7 @@
         <v>3000</v>
       </c>
       <c r="FB23" s="66"/>
-      <c r="FC23" s="725"/>
+      <c r="FC23" s="700"/>
       <c r="FD23" s="152" t="s">
         <v>2153</v>
       </c>
@@ -53524,10 +53527,10 @@
       <c r="HI23" s="99">
         <v>2000</v>
       </c>
-      <c r="HJ23" s="706" t="s">
+      <c r="HJ23" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="HK23" s="706"/>
+      <c r="HK23" s="703"/>
       <c r="HL23" s="152" t="s">
         <v>2158</v>
       </c>
@@ -53554,10 +53557,10 @@
         <f>5002+10000+10000+5000</f>
         <v>30002</v>
       </c>
-      <c r="HV23" s="706" t="s">
+      <c r="HV23" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="HW23" s="706"/>
+      <c r="HW23" s="703"/>
       <c r="HX23" s="169" t="s">
         <v>2160</v>
       </c>
@@ -53925,62 +53928,62 @@
       <c r="NE23" s="288"/>
     </row>
     <row r="24" spans="1:372">
-      <c r="A24" s="715" t="s">
+      <c r="A24" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="B24" s="715"/>
+      <c r="B24" s="704"/>
       <c r="E24" s="565" t="s">
         <v>271</v>
       </c>
       <c r="F24" s="63"/>
-      <c r="G24" s="715" t="s">
+      <c r="G24" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="H24" s="715"/>
+      <c r="H24" s="704"/>
       <c r="K24" s="71" t="s">
         <v>1518</v>
       </c>
       <c r="L24" s="66">
         <v>0</v>
       </c>
-      <c r="M24" s="714"/>
-      <c r="N24" s="714"/>
+      <c r="M24" s="710"/>
+      <c r="N24" s="710"/>
       <c r="Q24" s="71" t="s">
         <v>1617</v>
       </c>
       <c r="R24" s="14">
         <v>0</v>
       </c>
-      <c r="S24" s="714"/>
-      <c r="T24" s="714"/>
+      <c r="S24" s="710"/>
+      <c r="T24" s="710"/>
       <c r="W24" s="71" t="s">
         <v>2184</v>
       </c>
       <c r="X24" s="14">
         <v>910.17</v>
       </c>
-      <c r="Y24" s="714"/>
-      <c r="Z24" s="714"/>
+      <c r="Y24" s="710"/>
+      <c r="Z24" s="710"/>
       <c r="AC24" s="78" t="s">
         <v>2185</v>
       </c>
       <c r="AD24" s="14">
         <v>90</v>
       </c>
-      <c r="AE24" s="715" t="s">
+      <c r="AE24" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="AF24" s="715"/>
+      <c r="AF24" s="704"/>
       <c r="AI24" s="77" t="s">
         <v>2186</v>
       </c>
       <c r="AJ24" s="14">
         <v>30</v>
       </c>
-      <c r="AK24" s="715" t="s">
+      <c r="AK24" s="704" t="s">
         <v>2092</v>
       </c>
-      <c r="AL24" s="715"/>
+      <c r="AL24" s="704"/>
       <c r="AO24" s="71" t="s">
         <v>1518</v>
       </c>
@@ -54008,60 +54011,60 @@
       <c r="BF24" s="66">
         <v>54.83</v>
       </c>
-      <c r="BG24" s="715"/>
-      <c r="BH24" s="715"/>
+      <c r="BG24" s="704"/>
+      <c r="BH24" s="704"/>
       <c r="BK24" s="94" t="s">
         <v>2188</v>
       </c>
       <c r="BL24" s="66">
         <v>48.54</v>
       </c>
-      <c r="BM24" s="715"/>
-      <c r="BN24" s="715"/>
+      <c r="BM24" s="704"/>
+      <c r="BN24" s="704"/>
       <c r="BQ24" s="94" t="s">
         <v>1919</v>
       </c>
       <c r="BR24" s="66">
         <v>50.15</v>
       </c>
-      <c r="BS24" s="715" t="s">
+      <c r="BS24" s="704" t="s">
         <v>2189</v>
       </c>
-      <c r="BT24" s="715"/>
+      <c r="BT24" s="704"/>
       <c r="BW24" s="94" t="s">
         <v>1919</v>
       </c>
       <c r="BX24" s="66">
         <v>48.54</v>
       </c>
-      <c r="BY24" s="715"/>
-      <c r="BZ24" s="715"/>
+      <c r="BY24" s="704"/>
+      <c r="BZ24" s="704"/>
       <c r="CC24" s="94" t="s">
         <v>1919</v>
       </c>
       <c r="CD24" s="66">
         <v>142.91</v>
       </c>
-      <c r="CE24" s="715"/>
-      <c r="CF24" s="715"/>
+      <c r="CE24" s="704"/>
+      <c r="CF24" s="704"/>
       <c r="CI24" s="94" t="s">
         <v>2190</v>
       </c>
       <c r="CJ24" s="66">
         <v>35.049999999999997</v>
       </c>
-      <c r="CK24" s="714"/>
-      <c r="CL24" s="714"/>
+      <c r="CK24" s="710"/>
+      <c r="CL24" s="710"/>
       <c r="CO24" s="94" t="s">
         <v>1867</v>
       </c>
       <c r="CP24" s="66">
         <v>153.41</v>
       </c>
-      <c r="CQ24" s="714" t="s">
+      <c r="CQ24" s="710" t="s">
         <v>2191</v>
       </c>
-      <c r="CR24" s="714"/>
+      <c r="CR24" s="710"/>
       <c r="CU24" s="94" t="s">
         <v>2144</v>
       </c>
@@ -54177,7 +54180,7 @@
       <c r="EU24" s="99">
         <v>0</v>
       </c>
-      <c r="EW24" s="725"/>
+      <c r="EW24" s="700"/>
       <c r="EX24" s="152" t="s">
         <v>2205</v>
       </c>
@@ -54718,14 +54721,14 @@
       <c r="NE24" s="50"/>
     </row>
     <row r="25" spans="1:372">
-      <c r="A25" s="714"/>
-      <c r="B25" s="714"/>
+      <c r="A25" s="710"/>
+      <c r="B25" s="710"/>
       <c r="E25" s="564" t="s">
         <v>386</v>
       </c>
       <c r="F25" s="58"/>
-      <c r="G25" s="714"/>
-      <c r="H25" s="714"/>
+      <c r="G25" s="710"/>
+      <c r="H25" s="710"/>
       <c r="K25" s="71" t="s">
         <v>2240</v>
       </c>
@@ -54733,28 +54736,28 @@
         <f>910+40</f>
         <v>950</v>
       </c>
-      <c r="M25" s="714"/>
-      <c r="N25" s="714"/>
+      <c r="M25" s="710"/>
+      <c r="N25" s="710"/>
       <c r="Q25" s="71" t="s">
         <v>1680</v>
       </c>
       <c r="R25" s="14">
         <v>0</v>
       </c>
-      <c r="S25" s="714"/>
-      <c r="T25" s="714"/>
+      <c r="S25" s="710"/>
+      <c r="T25" s="710"/>
       <c r="W25" s="72" t="s">
         <v>2241</v>
       </c>
       <c r="X25" s="14">
         <v>110.58</v>
       </c>
-      <c r="Y25" s="714"/>
-      <c r="Z25" s="714"/>
-      <c r="AE25" s="714"/>
-      <c r="AF25" s="714"/>
-      <c r="AK25" s="714"/>
-      <c r="AL25" s="714"/>
+      <c r="Y25" s="710"/>
+      <c r="Z25" s="710"/>
+      <c r="AE25" s="710"/>
+      <c r="AF25" s="710"/>
+      <c r="AK25" s="710"/>
+      <c r="AL25" s="710"/>
       <c r="AO25" s="72" t="s">
         <v>2242</v>
       </c>
@@ -54768,12 +54771,12 @@
       <c r="AV25" s="66">
         <v>172.57</v>
       </c>
-      <c r="AW25" s="714"/>
-      <c r="AX25" s="714"/>
+      <c r="AW25" s="710"/>
+      <c r="AX25" s="710"/>
       <c r="AY25" s="72"/>
       <c r="AZ25" s="66"/>
-      <c r="BA25" s="714"/>
-      <c r="BB25" s="714"/>
+      <c r="BA25" s="710"/>
+      <c r="BB25" s="710"/>
       <c r="BE25" s="72" t="s">
         <v>1547</v>
       </c>
@@ -54781,8 +54784,8 @@
         <f>6.5*2</f>
         <v>13</v>
       </c>
-      <c r="BG25" s="714"/>
-      <c r="BH25" s="714"/>
+      <c r="BG25" s="710"/>
+      <c r="BH25" s="710"/>
       <c r="BK25" s="94" t="s">
         <v>1547</v>
       </c>
@@ -54790,32 +54793,32 @@
         <f>6.5*2</f>
         <v>13</v>
       </c>
-      <c r="BM25" s="714"/>
-      <c r="BN25" s="714"/>
+      <c r="BM25" s="710"/>
+      <c r="BN25" s="710"/>
       <c r="BQ25" s="94" t="s">
         <v>1547</v>
       </c>
       <c r="BR25" s="66">
         <v>13</v>
       </c>
-      <c r="BS25" s="714"/>
-      <c r="BT25" s="714"/>
+      <c r="BS25" s="710"/>
+      <c r="BT25" s="710"/>
       <c r="BW25" s="94" t="s">
         <v>1547</v>
       </c>
       <c r="BX25" s="66">
         <v>13</v>
       </c>
-      <c r="BY25" s="714"/>
-      <c r="BZ25" s="714"/>
+      <c r="BY25" s="710"/>
+      <c r="BZ25" s="710"/>
       <c r="CC25" s="94" t="s">
         <v>1547</v>
       </c>
       <c r="CD25" s="66">
         <v>13</v>
       </c>
-      <c r="CE25" s="714"/>
-      <c r="CF25" s="714"/>
+      <c r="CE25" s="710"/>
+      <c r="CF25" s="710"/>
       <c r="CI25" s="94" t="s">
         <v>1547</v>
       </c>
@@ -54891,10 +54894,10 @@
       <c r="DV25" s="97">
         <v>5000</v>
       </c>
-      <c r="DY25" s="717" t="s">
+      <c r="DY25" s="716" t="s">
         <v>2150</v>
       </c>
-      <c r="DZ25" s="718"/>
+      <c r="DZ25" s="717"/>
       <c r="EA25" s="21" t="s">
         <v>2249</v>
       </c>
@@ -54923,17 +54926,17 @@
       <c r="EO25" s="99">
         <v>0</v>
       </c>
-      <c r="ER25" s="716" t="s">
+      <c r="ER25" s="715" t="s">
         <v>2150</v>
       </c>
-      <c r="ES25" s="716"/>
+      <c r="ES25" s="715"/>
       <c r="ET25" s="54" t="s">
         <v>1811</v>
       </c>
       <c r="EU25" s="99">
         <v>20000</v>
       </c>
-      <c r="EW25" s="725"/>
+      <c r="EW25" s="700"/>
       <c r="EX25" s="152" t="s">
         <v>2252</v>
       </c>
@@ -55134,10 +55137,10 @@
       <c r="IA25" s="99">
         <v>-13000</v>
       </c>
-      <c r="IB25" s="706" t="s">
+      <c r="IB25" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="IC25" s="706"/>
+      <c r="IC25" s="703"/>
       <c r="ID25" s="169" t="s">
         <v>2115</v>
       </c>
@@ -55444,41 +55447,41 @@
       <c r="NE25" s="50"/>
     </row>
     <row r="26" spans="1:372">
-      <c r="A26" s="714"/>
-      <c r="B26" s="714"/>
+      <c r="A26" s="710"/>
+      <c r="B26" s="710"/>
       <c r="F26" s="67"/>
-      <c r="G26" s="714"/>
-      <c r="H26" s="714"/>
-      <c r="M26" s="719" t="s">
+      <c r="G26" s="710"/>
+      <c r="H26" s="710"/>
+      <c r="M26" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="N26" s="714"/>
+      <c r="N26" s="710"/>
       <c r="Q26" s="71" t="s">
         <v>1737</v>
       </c>
       <c r="R26" s="14">
         <v>0</v>
       </c>
-      <c r="S26" s="719" t="s">
+      <c r="S26" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="T26" s="714"/>
+      <c r="T26" s="710"/>
       <c r="W26" s="72" t="s">
         <v>1919</v>
       </c>
       <c r="X26" s="14">
         <v>60.75</v>
       </c>
-      <c r="Y26" s="714"/>
-      <c r="Z26" s="714"/>
+      <c r="Y26" s="710"/>
+      <c r="Z26" s="710"/>
       <c r="AC26" s="21" t="s">
         <v>2285</v>
       </c>
       <c r="AD26" s="21"/>
-      <c r="AE26" s="719" t="s">
+      <c r="AE26" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="AF26" s="714"/>
+      <c r="AF26" s="710"/>
       <c r="AI26" s="66" t="s">
         <v>2286</v>
       </c>
@@ -55692,10 +55695,10 @@
       <c r="EU26" s="99">
         <v>10000</v>
       </c>
-      <c r="EX26" s="716" t="s">
+      <c r="EX26" s="715" t="s">
         <v>2150</v>
       </c>
-      <c r="EY26" s="716"/>
+      <c r="EY26" s="715"/>
       <c r="EZ26" s="54" t="s">
         <v>1811</v>
       </c>
@@ -55851,10 +55854,10 @@
         <v>2299</v>
       </c>
       <c r="HO26" s="102"/>
-      <c r="HP26" s="706" t="s">
+      <c r="HP26" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="HQ26" s="706"/>
+      <c r="HQ26" s="703"/>
       <c r="HR26" s="152" t="s">
         <v>2307</v>
       </c>
@@ -56181,14 +56184,14 @@
       <c r="NE26" s="50"/>
     </row>
     <row r="27" spans="1:372" ht="12.75" customHeight="1">
-      <c r="A27" s="714"/>
-      <c r="B27" s="714"/>
+      <c r="A27" s="710"/>
+      <c r="B27" s="710"/>
       <c r="E27" s="567" t="s">
         <v>418</v>
       </c>
       <c r="F27" s="67"/>
-      <c r="G27" s="714"/>
-      <c r="H27" s="714"/>
+      <c r="G27" s="710"/>
+      <c r="H27" s="710"/>
       <c r="K27" s="72" t="s">
         <v>2333</v>
       </c>
@@ -56196,30 +56199,30 @@
         <f>60</f>
         <v>60</v>
       </c>
-      <c r="M27" s="719" t="s">
+      <c r="M27" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="N27" s="714"/>
+      <c r="N27" s="710"/>
       <c r="Q27" s="71" t="s">
         <v>2335</v>
       </c>
       <c r="R27" s="66">
         <v>200</v>
       </c>
-      <c r="S27" s="719" t="s">
+      <c r="S27" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="T27" s="714"/>
+      <c r="T27" s="710"/>
       <c r="W27" s="72" t="s">
         <v>1987</v>
       </c>
       <c r="X27" s="14">
         <v>61.35</v>
       </c>
-      <c r="Y27" s="719" t="s">
+      <c r="Y27" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="Z27" s="714"/>
+      <c r="Z27" s="710"/>
       <c r="AC27" s="21" t="s">
         <v>2336</v>
       </c>
@@ -56227,10 +56230,10 @@
         <f>53+207+63</f>
         <v>323</v>
       </c>
-      <c r="AE27" s="719" t="s">
+      <c r="AE27" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="AF27" s="714"/>
+      <c r="AF27" s="710"/>
       <c r="AI27" s="14" t="s">
         <v>2337</v>
       </c>
@@ -56449,10 +56452,10 @@
       <c r="FA27" s="99">
         <v>11010</v>
       </c>
-      <c r="FD27" s="716" t="s">
+      <c r="FD27" s="715" t="s">
         <v>2356</v>
       </c>
-      <c r="FE27" s="716"/>
+      <c r="FE27" s="715"/>
       <c r="FF27" s="54" t="s">
         <v>1806</v>
       </c>
@@ -56956,48 +56959,48 @@
       <c r="NE27" s="50"/>
     </row>
     <row r="28" spans="1:372">
-      <c r="A28" s="719" t="s">
+      <c r="A28" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="B28" s="714"/>
+      <c r="B28" s="710"/>
       <c r="E28" s="567" t="s">
         <v>427</v>
       </c>
       <c r="F28" s="67"/>
-      <c r="G28" s="719" t="s">
+      <c r="G28" s="714" t="s">
         <v>372</v>
       </c>
-      <c r="H28" s="714"/>
+      <c r="H28" s="710"/>
       <c r="K28" s="72" t="s">
         <v>1987</v>
       </c>
       <c r="L28" s="14">
         <v>0</v>
       </c>
-      <c r="M28" s="720" t="s">
+      <c r="M28" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="N28" s="720"/>
+      <c r="N28" s="699"/>
       <c r="Q28" s="71" t="s">
         <v>2184</v>
       </c>
       <c r="R28" s="14">
         <v>0</v>
       </c>
-      <c r="S28" s="720" t="s">
+      <c r="S28" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="T28" s="720"/>
+      <c r="T28" s="699"/>
       <c r="W28" s="72" t="s">
         <v>2042</v>
       </c>
       <c r="X28" s="14">
         <v>64</v>
       </c>
-      <c r="Y28" s="719" t="s">
+      <c r="Y28" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="Z28" s="714"/>
+      <c r="Z28" s="710"/>
       <c r="AC28" s="21" t="s">
         <v>2394</v>
       </c>
@@ -57005,10 +57008,10 @@
         <f>63+46</f>
         <v>109</v>
       </c>
-      <c r="AE28" s="720" t="s">
+      <c r="AE28" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="AF28" s="720"/>
+      <c r="AF28" s="699"/>
       <c r="AI28" s="14" t="s">
         <v>2395</v>
       </c>
@@ -57188,10 +57191,10 @@
       </c>
       <c r="EF28" s="21"/>
       <c r="EG28" s="165"/>
-      <c r="EL28" s="716" t="s">
+      <c r="EL28" s="715" t="s">
         <v>2150</v>
       </c>
-      <c r="EM28" s="716"/>
+      <c r="EM28" s="715"/>
       <c r="EN28" s="74"/>
       <c r="EO28" s="96"/>
       <c r="ER28" s="21" t="s">
@@ -57460,10 +57463,10 @@
       </c>
       <c r="IW28" s="51"/>
       <c r="IX28" s="74"/>
-      <c r="IZ28" s="706" t="s">
+      <c r="IZ28" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="JA28" s="706"/>
+      <c r="JA28" s="703"/>
       <c r="JB28" s="152" t="s">
         <v>2430</v>
       </c>
@@ -57694,52 +57697,52 @@
       </c>
     </row>
     <row r="29" spans="1:372">
-      <c r="A29" s="719" t="s">
+      <c r="A29" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="B29" s="714"/>
+      <c r="B29" s="710"/>
       <c r="E29" s="567" t="s">
         <v>431</v>
       </c>
       <c r="F29" s="67"/>
-      <c r="G29" s="719" t="s">
+      <c r="G29" s="714" t="s">
         <v>2334</v>
       </c>
-      <c r="H29" s="714"/>
+      <c r="H29" s="710"/>
       <c r="K29" s="72" t="s">
         <v>2042</v>
       </c>
       <c r="L29" s="14">
         <v>64</v>
       </c>
-      <c r="M29" s="714" t="s">
+      <c r="M29" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="N29" s="714"/>
-      <c r="S29" s="714" t="s">
+      <c r="N29" s="710"/>
+      <c r="S29" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="T29" s="714"/>
+      <c r="T29" s="710"/>
       <c r="W29" s="72" t="s">
         <v>2093</v>
       </c>
       <c r="X29" s="14">
         <v>100.01</v>
       </c>
-      <c r="Y29" s="720" t="s">
+      <c r="Y29" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="Z29" s="720"/>
+      <c r="Z29" s="699"/>
       <c r="AC29" s="14" t="s">
         <v>2446</v>
       </c>
       <c r="AD29" s="14">
         <v>65</v>
       </c>
-      <c r="AE29" s="714" t="s">
+      <c r="AE29" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="AF29" s="714"/>
+      <c r="AF29" s="710"/>
       <c r="AK29" s="14" t="s">
         <v>300</v>
       </c>
@@ -57940,10 +57943,10 @@
       <c r="FG29" s="99">
         <v>10010</v>
       </c>
-      <c r="FJ29" s="716" t="s">
+      <c r="FJ29" s="715" t="s">
         <v>2356</v>
       </c>
-      <c r="FK29" s="716"/>
+      <c r="FK29" s="715"/>
       <c r="FL29" s="54" t="s">
         <v>1811</v>
       </c>
@@ -58421,52 +58424,52 @@
       </c>
     </row>
     <row r="30" spans="1:372">
-      <c r="A30" s="720" t="s">
+      <c r="A30" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="720"/>
+      <c r="B30" s="699"/>
       <c r="E30" s="567" t="s">
         <v>2489</v>
       </c>
       <c r="F30" s="58"/>
-      <c r="G30" s="720" t="s">
+      <c r="G30" s="699" t="s">
         <v>197</v>
       </c>
-      <c r="H30" s="720"/>
+      <c r="H30" s="699"/>
       <c r="K30" s="72" t="s">
         <v>2093</v>
       </c>
       <c r="L30" s="14">
         <v>50.01</v>
       </c>
-      <c r="M30" s="724" t="s">
+      <c r="M30" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="N30" s="724"/>
+      <c r="N30" s="711"/>
       <c r="Q30" s="72" t="s">
         <v>1855</v>
       </c>
       <c r="R30" s="14">
         <v>26</v>
       </c>
-      <c r="S30" s="724" t="s">
+      <c r="S30" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="T30" s="724"/>
-      <c r="Y30" s="714" t="s">
+      <c r="T30" s="711"/>
+      <c r="Y30" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="Z30" s="714"/>
+      <c r="Z30" s="710"/>
       <c r="AC30" s="14" t="s">
         <v>2491</v>
       </c>
       <c r="AD30" s="14">
         <v>10</v>
       </c>
-      <c r="AE30" s="724" t="s">
+      <c r="AE30" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="AF30" s="724"/>
+      <c r="AF30" s="711"/>
       <c r="AK30" s="82" t="s">
         <v>2490</v>
       </c>
@@ -59147,44 +59150,44 @@
       <c r="NE30" s="43"/>
     </row>
     <row r="31" spans="1:372" ht="12.75" customHeight="1">
-      <c r="A31" s="714" t="s">
+      <c r="A31" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="B31" s="714"/>
+      <c r="B31" s="710"/>
       <c r="E31" s="58"/>
       <c r="F31" s="58"/>
-      <c r="G31" s="714" t="s">
+      <c r="G31" s="710" t="s">
         <v>300</v>
       </c>
-      <c r="H31" s="714"/>
-      <c r="M31" s="715" t="s">
+      <c r="H31" s="710"/>
+      <c r="M31" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="N31" s="715"/>
+      <c r="N31" s="704"/>
       <c r="Q31" s="72" t="s">
         <v>1919</v>
       </c>
       <c r="R31" s="14">
         <v>55</v>
       </c>
-      <c r="S31" s="715" t="s">
+      <c r="S31" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="T31" s="715"/>
+      <c r="T31" s="704"/>
       <c r="W31" s="73" t="s">
         <v>2540</v>
       </c>
       <c r="X31" s="73">
         <v>0</v>
       </c>
-      <c r="Y31" s="724" t="s">
+      <c r="Y31" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="Z31" s="724"/>
-      <c r="AE31" s="715" t="s">
+      <c r="Z31" s="711"/>
+      <c r="AE31" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="AF31" s="715"/>
+      <c r="AF31" s="704"/>
       <c r="AK31" s="66" t="s">
         <v>363</v>
       </c>
@@ -59315,10 +59318,10 @@
       <c r="DN31" s="62">
         <v>5</v>
       </c>
-      <c r="DO31" s="731" t="s">
+      <c r="DO31" s="709" t="s">
         <v>2549</v>
       </c>
-      <c r="DP31" s="731"/>
+      <c r="DP31" s="709"/>
       <c r="DQ31" s="66"/>
       <c r="DS31" s="123" t="s">
         <v>2550</v>
@@ -59840,50 +59843,50 @@
       </c>
     </row>
     <row r="32" spans="1:372">
-      <c r="A32" s="724" t="s">
+      <c r="A32" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="B32" s="724"/>
+      <c r="B32" s="711"/>
       <c r="C32" s="69"/>
       <c r="D32" s="69"/>
       <c r="E32" s="69"/>
       <c r="F32" s="69"/>
-      <c r="G32" s="724" t="s">
+      <c r="G32" s="711" t="s">
         <v>2490</v>
       </c>
-      <c r="H32" s="724"/>
+      <c r="H32" s="711"/>
       <c r="K32" s="73" t="s">
         <v>2589</v>
       </c>
       <c r="L32" s="73"/>
-      <c r="M32" s="721" t="s">
+      <c r="M32" s="705" t="s">
         <v>2574</v>
       </c>
-      <c r="N32" s="721"/>
+      <c r="N32" s="705"/>
       <c r="Q32" s="72" t="s">
         <v>1987</v>
       </c>
       <c r="R32" s="14">
         <v>77.239999999999995</v>
       </c>
-      <c r="S32" s="721" t="s">
+      <c r="S32" s="705" t="s">
         <v>2574</v>
       </c>
-      <c r="T32" s="721"/>
-      <c r="Y32" s="715" t="s">
+      <c r="T32" s="705"/>
+      <c r="Y32" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="Z32" s="715"/>
+      <c r="Z32" s="704"/>
       <c r="AC32" s="574" t="s">
         <v>1395</v>
       </c>
       <c r="AD32" s="14">
         <v>350</v>
       </c>
-      <c r="AE32" s="721" t="s">
+      <c r="AE32" s="705" t="s">
         <v>2574</v>
       </c>
-      <c r="AF32" s="721"/>
+      <c r="AF32" s="705"/>
       <c r="AI32" s="574" t="s">
         <v>1395</v>
       </c>
@@ -59977,10 +59980,10 @@
         <v>2447</v>
       </c>
       <c r="CX32" s="106"/>
-      <c r="DA32" s="722" t="s">
+      <c r="DA32" s="712" t="s">
         <v>2478</v>
       </c>
-      <c r="DB32" s="723"/>
+      <c r="DB32" s="713"/>
       <c r="DC32" s="54" t="s">
         <v>197</v>
       </c>
@@ -60231,10 +60234,10 @@
       <c r="IL32" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="IN32" s="706" t="s">
+      <c r="IN32" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="IO32" s="706"/>
+      <c r="IO32" s="703"/>
       <c r="IP32" s="152" t="s">
         <v>2621</v>
       </c>
@@ -60485,18 +60488,18 @@
       </c>
     </row>
     <row r="33" spans="1:369">
-      <c r="A33" s="715" t="s">
+      <c r="A33" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="B33" s="715"/>
+      <c r="B33" s="704"/>
       <c r="E33" s="575" t="s">
         <v>455</v>
       </c>
       <c r="F33" s="58"/>
-      <c r="G33" s="715" t="s">
+      <c r="G33" s="704" t="s">
         <v>363</v>
       </c>
-      <c r="H33" s="715"/>
+      <c r="H33" s="704"/>
       <c r="K33" s="73" t="s">
         <v>2639</v>
       </c>
@@ -60515,10 +60518,10 @@
       <c r="X33" s="77">
         <v>283</v>
       </c>
-      <c r="Y33" s="721" t="s">
+      <c r="Y33" s="705" t="s">
         <v>2574</v>
       </c>
-      <c r="Z33" s="721"/>
+      <c r="Z33" s="705"/>
       <c r="AC33" s="564" t="s">
         <v>2641</v>
       </c>
@@ -61646,16 +61649,16 @@
       </c>
     </row>
     <row r="35" spans="1:369" ht="14.25" customHeight="1">
-      <c r="A35" s="728"/>
-      <c r="B35" s="728"/>
+      <c r="A35" s="706"/>
+      <c r="B35" s="706"/>
       <c r="E35" s="570" t="s">
         <v>493</v>
       </c>
       <c r="F35" s="58">
         <v>250</v>
       </c>
-      <c r="G35" s="728"/>
-      <c r="H35" s="728"/>
+      <c r="G35" s="706"/>
+      <c r="H35" s="706"/>
       <c r="W35" s="77" t="s">
         <v>2743</v>
       </c>
@@ -62312,10 +62315,10 @@
         <v>2334</v>
       </c>
       <c r="DP36" s="62"/>
-      <c r="DS36" s="729" t="s">
+      <c r="DS36" s="707" t="s">
         <v>2150</v>
       </c>
-      <c r="DT36" s="730"/>
+      <c r="DT36" s="708"/>
       <c r="DU36" s="564" t="s">
         <v>2554</v>
       </c>
@@ -63799,10 +63802,10 @@
       <c r="DH39" s="62">
         <v>32.200000000000003</v>
       </c>
-      <c r="DI39" s="731" t="s">
+      <c r="DI39" s="709" t="s">
         <v>2549</v>
       </c>
-      <c r="DJ39" s="731"/>
+      <c r="DJ39" s="709"/>
       <c r="DM39" s="127" t="s">
         <v>2753</v>
       </c>
@@ -64282,10 +64285,10 @@
       <c r="IE40" s="155" t="s">
         <v>2626</v>
       </c>
-      <c r="IH40" s="706" t="s">
+      <c r="IH40" s="703" t="s">
         <v>2118</v>
       </c>
-      <c r="II40" s="706"/>
+      <c r="II40" s="703"/>
       <c r="IJ40" s="203">
         <v>20</v>
       </c>
@@ -64702,10 +64705,10 @@
       <c r="KM41" s="243" t="s">
         <v>3000</v>
       </c>
-      <c r="KN41" s="720" t="s">
+      <c r="KN41" s="699" t="s">
         <v>2955</v>
       </c>
-      <c r="KO41" s="720"/>
+      <c r="KO41" s="699"/>
       <c r="KP41" s="152" t="s">
         <v>2429</v>
       </c>
@@ -66969,7 +66972,7 @@
       <c r="GU49" s="66">
         <v>60.6</v>
       </c>
-      <c r="GV49" s="726" t="s">
+      <c r="GV49" s="701" t="s">
         <v>3203</v>
       </c>
       <c r="GZ49" s="14" t="s">
@@ -67183,7 +67186,7 @@
       <c r="GU50" s="66">
         <v>14.9</v>
       </c>
-      <c r="GV50" s="726"/>
+      <c r="GV50" s="701"/>
       <c r="GZ50" s="183" t="s">
         <v>3226</v>
       </c>
@@ -67361,7 +67364,7 @@
       <c r="GU51" s="66">
         <v>55.29</v>
       </c>
-      <c r="GV51" s="726"/>
+      <c r="GV51" s="701"/>
       <c r="GZ51" s="14" t="s">
         <v>3101</v>
       </c>
@@ -67512,7 +67515,7 @@
         <v>38.9</v>
       </c>
       <c r="GU52" s="66"/>
-      <c r="GV52" s="726"/>
+      <c r="GV52" s="701"/>
       <c r="HF52" s="54"/>
       <c r="HX52" s="216" t="s">
         <v>3261</v>
@@ -68465,6 +68468,252 @@
     </row>
   </sheetData>
   <mergeCells count="270">
+    <mergeCell ref="NB1:NC1"/>
+    <mergeCell ref="NG13:NG14"/>
+    <mergeCell ref="NF16:NG16"/>
+    <mergeCell ref="NH13:NH14"/>
+    <mergeCell ref="MV1:MW1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BK1:BL1"/>
+    <mergeCell ref="BM1:BN1"/>
+    <mergeCell ref="BO1:BP1"/>
+    <mergeCell ref="BQ1:BR1"/>
+    <mergeCell ref="BS1:BT1"/>
+    <mergeCell ref="BU1:BV1"/>
+    <mergeCell ref="BW1:BX1"/>
+    <mergeCell ref="BY1:BZ1"/>
+    <mergeCell ref="CA1:CB1"/>
+    <mergeCell ref="CC1:CD1"/>
+    <mergeCell ref="CE1:CF1"/>
+    <mergeCell ref="CG1:CH1"/>
+    <mergeCell ref="CI1:CJ1"/>
+    <mergeCell ref="CK1:CL1"/>
+    <mergeCell ref="CM1:CN1"/>
+    <mergeCell ref="CO1:CP1"/>
+    <mergeCell ref="CQ1:CR1"/>
+    <mergeCell ref="CS1:CT1"/>
+    <mergeCell ref="CU1:CV1"/>
+    <mergeCell ref="CW1:CX1"/>
+    <mergeCell ref="CY1:CZ1"/>
+    <mergeCell ref="DA1:DB1"/>
+    <mergeCell ref="DC1:DD1"/>
+    <mergeCell ref="DE1:DF1"/>
+    <mergeCell ref="DG1:DH1"/>
+    <mergeCell ref="DI1:DJ1"/>
+    <mergeCell ref="DK1:DL1"/>
+    <mergeCell ref="DM1:DN1"/>
+    <mergeCell ref="DO1:DP1"/>
+    <mergeCell ref="DQ1:DR1"/>
+    <mergeCell ref="DS1:DT1"/>
+    <mergeCell ref="DU1:DV1"/>
+    <mergeCell ref="DW1:DX1"/>
+    <mergeCell ref="DY1:DZ1"/>
+    <mergeCell ref="EA1:EB1"/>
+    <mergeCell ref="EC1:ED1"/>
+    <mergeCell ref="EE1:EF1"/>
+    <mergeCell ref="EH1:EI1"/>
+    <mergeCell ref="EJ1:EK1"/>
+    <mergeCell ref="EL1:EM1"/>
+    <mergeCell ref="EN1:EO1"/>
+    <mergeCell ref="EP1:EQ1"/>
+    <mergeCell ref="ER1:ES1"/>
+    <mergeCell ref="ET1:EU1"/>
+    <mergeCell ref="EV1:EW1"/>
+    <mergeCell ref="EX1:EY1"/>
+    <mergeCell ref="EZ1:FA1"/>
+    <mergeCell ref="FB1:FC1"/>
+    <mergeCell ref="FD1:FE1"/>
+    <mergeCell ref="FF1:FG1"/>
+    <mergeCell ref="FH1:FI1"/>
+    <mergeCell ref="FJ1:FK1"/>
+    <mergeCell ref="FL1:FM1"/>
+    <mergeCell ref="FN1:FO1"/>
+    <mergeCell ref="FP1:FQ1"/>
+    <mergeCell ref="FR1:FS1"/>
+    <mergeCell ref="FT1:FU1"/>
+    <mergeCell ref="FV1:FW1"/>
+    <mergeCell ref="FX1:FY1"/>
+    <mergeCell ref="FZ1:GA1"/>
+    <mergeCell ref="GB1:GC1"/>
+    <mergeCell ref="GD1:GE1"/>
+    <mergeCell ref="GF1:GG1"/>
+    <mergeCell ref="GH1:GI1"/>
+    <mergeCell ref="GJ1:GK1"/>
+    <mergeCell ref="GL1:GM1"/>
+    <mergeCell ref="GN1:GO1"/>
+    <mergeCell ref="GP1:GQ1"/>
+    <mergeCell ref="GR1:GS1"/>
+    <mergeCell ref="GT1:GU1"/>
+    <mergeCell ref="GV1:GW1"/>
+    <mergeCell ref="GX1:GY1"/>
+    <mergeCell ref="GZ1:HA1"/>
+    <mergeCell ref="HB1:HC1"/>
+    <mergeCell ref="HD1:HE1"/>
+    <mergeCell ref="HF1:HG1"/>
+    <mergeCell ref="HH1:HI1"/>
+    <mergeCell ref="HJ1:HK1"/>
+    <mergeCell ref="HL1:HM1"/>
+    <mergeCell ref="HN1:HO1"/>
+    <mergeCell ref="HP1:HQ1"/>
+    <mergeCell ref="HR1:HS1"/>
+    <mergeCell ref="HT1:HU1"/>
+    <mergeCell ref="HV1:HW1"/>
+    <mergeCell ref="HX1:HY1"/>
+    <mergeCell ref="HZ1:IA1"/>
+    <mergeCell ref="JF1:JG1"/>
+    <mergeCell ref="JH1:JI1"/>
+    <mergeCell ref="JJ1:JK1"/>
+    <mergeCell ref="IB1:IC1"/>
+    <mergeCell ref="ID1:IE1"/>
+    <mergeCell ref="IF1:IG1"/>
+    <mergeCell ref="IH1:II1"/>
+    <mergeCell ref="IJ1:IK1"/>
+    <mergeCell ref="IL1:IM1"/>
+    <mergeCell ref="IN1:IO1"/>
+    <mergeCell ref="IP1:IQ1"/>
+    <mergeCell ref="IR1:IS1"/>
+    <mergeCell ref="LR1:LS1"/>
+    <mergeCell ref="LX1:LY1"/>
+    <mergeCell ref="MD1:ME1"/>
+    <mergeCell ref="MJ1:MK1"/>
+    <mergeCell ref="MP1:MQ1"/>
+    <mergeCell ref="DO14:DP14"/>
+    <mergeCell ref="HJ14:HK14"/>
+    <mergeCell ref="KD15:KE15"/>
+    <mergeCell ref="DI18:DJ18"/>
+    <mergeCell ref="JP1:JQ1"/>
+    <mergeCell ref="JV1:JW1"/>
+    <mergeCell ref="KB1:KC1"/>
+    <mergeCell ref="KH1:KI1"/>
+    <mergeCell ref="KN1:KO1"/>
+    <mergeCell ref="KT1:KU1"/>
+    <mergeCell ref="KZ1:LA1"/>
+    <mergeCell ref="LF1:LG1"/>
+    <mergeCell ref="LL1:LM1"/>
+    <mergeCell ref="IT1:IU1"/>
+    <mergeCell ref="IV1:IW1"/>
+    <mergeCell ref="IX1:IY1"/>
+    <mergeCell ref="IZ1:JA1"/>
+    <mergeCell ref="JB1:JC1"/>
+    <mergeCell ref="JD1:JE1"/>
+    <mergeCell ref="IT22:IU22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AK23:AL23"/>
+    <mergeCell ref="EE23:EF23"/>
+    <mergeCell ref="HJ23:HK23"/>
+    <mergeCell ref="HV23:HW23"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="AK24:AL24"/>
+    <mergeCell ref="BG24:BH24"/>
+    <mergeCell ref="BM24:BN24"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="BS24:BT24"/>
+    <mergeCell ref="BY24:BZ24"/>
+    <mergeCell ref="CE24:CF24"/>
+    <mergeCell ref="CK24:CL24"/>
+    <mergeCell ref="CQ24:CR24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="AE25:AF25"/>
+    <mergeCell ref="AK25:AL25"/>
+    <mergeCell ref="AW25:AX25"/>
+    <mergeCell ref="BA25:BB25"/>
+    <mergeCell ref="BG25:BH25"/>
+    <mergeCell ref="BM25:BN25"/>
+    <mergeCell ref="BS25:BT25"/>
+    <mergeCell ref="BY25:BZ25"/>
+    <mergeCell ref="CE25:CF25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="DY25:DZ25"/>
+    <mergeCell ref="ER25:ES25"/>
+    <mergeCell ref="IB25:IC25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="EX26:EY26"/>
+    <mergeCell ref="HP26:HQ26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="AE27:AF27"/>
+    <mergeCell ref="FD27:FE27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="AE28:AF28"/>
+    <mergeCell ref="EL28:EM28"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="AE32:AF32"/>
+    <mergeCell ref="DA32:DB32"/>
+    <mergeCell ref="IZ28:JA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="AE29:AF29"/>
+    <mergeCell ref="FJ29:FK29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="AE30:AF30"/>
     <mergeCell ref="KN41:KO41"/>
     <mergeCell ref="EW23:EW25"/>
     <mergeCell ref="FC21:FC23"/>
@@ -68489,252 +68738,6 @@
     <mergeCell ref="DO31:DP31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="AE32:AF32"/>
-    <mergeCell ref="DA32:DB32"/>
-    <mergeCell ref="IZ28:JA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="AE29:AF29"/>
-    <mergeCell ref="FJ29:FK29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="AE27:AF27"/>
-    <mergeCell ref="FD27:FE27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="AE28:AF28"/>
-    <mergeCell ref="EL28:EM28"/>
-    <mergeCell ref="DY25:DZ25"/>
-    <mergeCell ref="ER25:ES25"/>
-    <mergeCell ref="IB25:IC25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="EX26:EY26"/>
-    <mergeCell ref="HP26:HQ26"/>
-    <mergeCell ref="BS24:BT24"/>
-    <mergeCell ref="BY24:BZ24"/>
-    <mergeCell ref="CE24:CF24"/>
-    <mergeCell ref="CK24:CL24"/>
-    <mergeCell ref="CQ24:CR24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="AE25:AF25"/>
-    <mergeCell ref="AK25:AL25"/>
-    <mergeCell ref="AW25:AX25"/>
-    <mergeCell ref="BA25:BB25"/>
-    <mergeCell ref="BG25:BH25"/>
-    <mergeCell ref="BM25:BN25"/>
-    <mergeCell ref="BS25:BT25"/>
-    <mergeCell ref="BY25:BZ25"/>
-    <mergeCell ref="CE25:CF25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AK24:AL24"/>
-    <mergeCell ref="BG24:BH24"/>
-    <mergeCell ref="BM24:BN24"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="IT22:IU22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AK23:AL23"/>
-    <mergeCell ref="EE23:EF23"/>
-    <mergeCell ref="HJ23:HK23"/>
-    <mergeCell ref="HV23:HW23"/>
-    <mergeCell ref="LR1:LS1"/>
-    <mergeCell ref="LX1:LY1"/>
-    <mergeCell ref="MD1:ME1"/>
-    <mergeCell ref="MJ1:MK1"/>
-    <mergeCell ref="MP1:MQ1"/>
-    <mergeCell ref="DO14:DP14"/>
-    <mergeCell ref="HJ14:HK14"/>
-    <mergeCell ref="KD15:KE15"/>
-    <mergeCell ref="DI18:DJ18"/>
-    <mergeCell ref="JP1:JQ1"/>
-    <mergeCell ref="JV1:JW1"/>
-    <mergeCell ref="KB1:KC1"/>
-    <mergeCell ref="KH1:KI1"/>
-    <mergeCell ref="KN1:KO1"/>
-    <mergeCell ref="KT1:KU1"/>
-    <mergeCell ref="KZ1:LA1"/>
-    <mergeCell ref="LF1:LG1"/>
-    <mergeCell ref="LL1:LM1"/>
-    <mergeCell ref="IT1:IU1"/>
-    <mergeCell ref="IV1:IW1"/>
-    <mergeCell ref="IX1:IY1"/>
-    <mergeCell ref="IZ1:JA1"/>
-    <mergeCell ref="JB1:JC1"/>
-    <mergeCell ref="JD1:JE1"/>
-    <mergeCell ref="JH1:JI1"/>
-    <mergeCell ref="JJ1:JK1"/>
-    <mergeCell ref="IB1:IC1"/>
-    <mergeCell ref="ID1:IE1"/>
-    <mergeCell ref="IF1:IG1"/>
-    <mergeCell ref="IH1:II1"/>
-    <mergeCell ref="IJ1:IK1"/>
-    <mergeCell ref="IL1:IM1"/>
-    <mergeCell ref="IN1:IO1"/>
-    <mergeCell ref="IP1:IQ1"/>
-    <mergeCell ref="IR1:IS1"/>
-    <mergeCell ref="HL1:HM1"/>
-    <mergeCell ref="HN1:HO1"/>
-    <mergeCell ref="HP1:HQ1"/>
-    <mergeCell ref="HR1:HS1"/>
-    <mergeCell ref="HT1:HU1"/>
-    <mergeCell ref="HV1:HW1"/>
-    <mergeCell ref="HX1:HY1"/>
-    <mergeCell ref="HZ1:IA1"/>
-    <mergeCell ref="JF1:JG1"/>
-    <mergeCell ref="GT1:GU1"/>
-    <mergeCell ref="GV1:GW1"/>
-    <mergeCell ref="GX1:GY1"/>
-    <mergeCell ref="GZ1:HA1"/>
-    <mergeCell ref="HB1:HC1"/>
-    <mergeCell ref="HD1:HE1"/>
-    <mergeCell ref="HF1:HG1"/>
-    <mergeCell ref="HH1:HI1"/>
-    <mergeCell ref="HJ1:HK1"/>
-    <mergeCell ref="GB1:GC1"/>
-    <mergeCell ref="GD1:GE1"/>
-    <mergeCell ref="GF1:GG1"/>
-    <mergeCell ref="GH1:GI1"/>
-    <mergeCell ref="GJ1:GK1"/>
-    <mergeCell ref="GL1:GM1"/>
-    <mergeCell ref="GN1:GO1"/>
-    <mergeCell ref="GP1:GQ1"/>
-    <mergeCell ref="GR1:GS1"/>
-    <mergeCell ref="FJ1:FK1"/>
-    <mergeCell ref="FL1:FM1"/>
-    <mergeCell ref="FN1:FO1"/>
-    <mergeCell ref="FP1:FQ1"/>
-    <mergeCell ref="FR1:FS1"/>
-    <mergeCell ref="FT1:FU1"/>
-    <mergeCell ref="FV1:FW1"/>
-    <mergeCell ref="FX1:FY1"/>
-    <mergeCell ref="FZ1:GA1"/>
-    <mergeCell ref="ER1:ES1"/>
-    <mergeCell ref="ET1:EU1"/>
-    <mergeCell ref="EV1:EW1"/>
-    <mergeCell ref="EX1:EY1"/>
-    <mergeCell ref="EZ1:FA1"/>
-    <mergeCell ref="FB1:FC1"/>
-    <mergeCell ref="FD1:FE1"/>
-    <mergeCell ref="FF1:FG1"/>
-    <mergeCell ref="FH1:FI1"/>
-    <mergeCell ref="DY1:DZ1"/>
-    <mergeCell ref="EA1:EB1"/>
-    <mergeCell ref="EC1:ED1"/>
-    <mergeCell ref="EE1:EF1"/>
-    <mergeCell ref="EH1:EI1"/>
-    <mergeCell ref="EJ1:EK1"/>
-    <mergeCell ref="EL1:EM1"/>
-    <mergeCell ref="EN1:EO1"/>
-    <mergeCell ref="EP1:EQ1"/>
-    <mergeCell ref="DG1:DH1"/>
-    <mergeCell ref="DI1:DJ1"/>
-    <mergeCell ref="DK1:DL1"/>
-    <mergeCell ref="DM1:DN1"/>
-    <mergeCell ref="DO1:DP1"/>
-    <mergeCell ref="DQ1:DR1"/>
-    <mergeCell ref="DS1:DT1"/>
-    <mergeCell ref="DU1:DV1"/>
-    <mergeCell ref="DW1:DX1"/>
-    <mergeCell ref="CO1:CP1"/>
-    <mergeCell ref="CQ1:CR1"/>
-    <mergeCell ref="CS1:CT1"/>
-    <mergeCell ref="CU1:CV1"/>
-    <mergeCell ref="CW1:CX1"/>
-    <mergeCell ref="CY1:CZ1"/>
-    <mergeCell ref="DA1:DB1"/>
-    <mergeCell ref="DC1:DD1"/>
-    <mergeCell ref="DE1:DF1"/>
-    <mergeCell ref="BW1:BX1"/>
-    <mergeCell ref="BY1:BZ1"/>
-    <mergeCell ref="CA1:CB1"/>
-    <mergeCell ref="CC1:CD1"/>
-    <mergeCell ref="CE1:CF1"/>
-    <mergeCell ref="CG1:CH1"/>
-    <mergeCell ref="CI1:CJ1"/>
-    <mergeCell ref="CK1:CL1"/>
-    <mergeCell ref="CM1:CN1"/>
-    <mergeCell ref="BE1:BF1"/>
-    <mergeCell ref="BG1:BH1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BK1:BL1"/>
-    <mergeCell ref="BM1:BN1"/>
-    <mergeCell ref="BO1:BP1"/>
-    <mergeCell ref="BQ1:BR1"/>
-    <mergeCell ref="BS1:BT1"/>
-    <mergeCell ref="BU1:BV1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="NB1:NC1"/>
-    <mergeCell ref="NG13:NG14"/>
-    <mergeCell ref="NF16:NG16"/>
-    <mergeCell ref="NH13:NH14"/>
-    <mergeCell ref="MV1:MW1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>

</xml_diff>